<commit_message>
added data, master key updates
data up to 4/7/25 now in the folder. master key notes column updated with mishaps from the run so far. removeSessions column still needs to be updated.
</commit_message>
<xml_diff>
--- a/All Outputs/Exp_all_Run_all_exclusions/Behavior Tables/run_all_exp_ER_GroupStats.xlsx
+++ b/All Outputs/Exp_all_Run_all_exclusions/Behavior Tables/run_all_exp_ER_GroupStats.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="258" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="407" uniqueCount="23">
   <si>
     <t>Sex</t>
   </si>
@@ -127,7 +127,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q17"/>
+  <dimension ref="A1:Q45"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -421,45 +421,49 @@
         <v>4</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="D6" s="0">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E6" s="0">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F6" s="0">
-        <v>22.333333333333332</v>
+        <v>92.166666666666671</v>
       </c>
       <c r="G6" s="0">
-        <v>5.8404718226450774</v>
+        <v>38.300058021423993</v>
       </c>
       <c r="H6" s="0">
-        <v>11.333333333333334</v>
+        <v>11</v>
       </c>
       <c r="I6" s="0">
-        <v>2.9059326290271157</v>
+        <v>5.3789714010518157</v>
       </c>
       <c r="J6" s="0">
-        <v>11</v>
+        <v>39.5</v>
       </c>
       <c r="K6" s="0">
-        <v>0.57735026918962584</v>
+        <v>15.411575736006577</v>
       </c>
       <c r="L6" s="0">
-        <v>42.666666666666664</v>
+        <v>83.333333333333329</v>
       </c>
       <c r="M6" s="0">
-        <v>13.245544324203685</v>
-      </c>
-      <c r="N6" s="0"/>
-      <c r="O6" s="0"/>
+        <v>32.352915032669173</v>
+      </c>
+      <c r="N6" s="0">
+        <v>161.37142538471747</v>
+      </c>
+      <c r="O6" s="0">
+        <v>103.62554349065974</v>
+      </c>
       <c r="P6" s="0">
-        <v>0</v>
+        <v>216.24832893199013</v>
       </c>
       <c r="Q6" s="0">
-        <v>0</v>
+        <v>89.529740512532555</v>
       </c>
     </row>
     <row r="7">
@@ -470,49 +474,49 @@
         <v>4</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="D7" s="0">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E7" s="0">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F7" s="0">
-        <v>17.666666666666668</v>
+        <v>32.75</v>
       </c>
       <c r="G7" s="0">
-        <v>17.169093679567879</v>
+        <v>14.378079380315949</v>
       </c>
       <c r="H7" s="0">
-        <v>0.33333333333333331</v>
+        <v>5.25</v>
       </c>
       <c r="I7" s="0">
-        <v>0.33333333333333337</v>
+        <v>2.8686524130097508</v>
       </c>
       <c r="J7" s="0">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="K7" s="0">
-        <v>10.503967504392488</v>
+        <v>6.1237243569579451</v>
       </c>
       <c r="L7" s="0">
-        <v>66</v>
+        <v>36.5</v>
       </c>
       <c r="M7" s="0">
-        <v>23.797758998135379</v>
+        <v>16.132265804901678</v>
       </c>
       <c r="N7" s="0">
-        <v>147.12807692307683</v>
+        <v>257.74884313725494</v>
       </c>
       <c r="O7" s="0">
-        <v>124.50807692307683</v>
+        <v>162.82175183132367</v>
       </c>
       <c r="P7" s="0">
-        <v>59.720951008334417</v>
+        <v>83.270458655521409</v>
       </c>
       <c r="Q7" s="0">
-        <v>57.017462445790393</v>
+        <v>30.552435766713579</v>
       </c>
     </row>
     <row r="8">
@@ -523,49 +527,49 @@
         <v>4</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="D8" s="0">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E8" s="0">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F8" s="0">
-        <v>15.666666666666666</v>
+        <v>46.5</v>
       </c>
       <c r="G8" s="0">
-        <v>7.4236858171066959</v>
+        <v>11.84271928232701</v>
       </c>
       <c r="H8" s="0">
-        <v>6.666666666666667</v>
+        <v>17</v>
       </c>
       <c r="I8" s="0">
-        <v>6.666666666666667</v>
+        <v>5.1153364177409353</v>
       </c>
       <c r="J8" s="0">
-        <v>9.6666666666666661</v>
+        <v>24.25</v>
       </c>
       <c r="K8" s="0">
-        <v>4.4845413490245702</v>
+        <v>5.1861192941672032</v>
       </c>
       <c r="L8" s="0">
-        <v>62</v>
+        <v>32</v>
       </c>
       <c r="M8" s="0">
-        <v>15.176736583776281</v>
+        <v>7.2915476180757857</v>
       </c>
       <c r="N8" s="0">
-        <v>50.378703703703508</v>
+        <v>117.15584108946607</v>
       </c>
       <c r="O8" s="0">
-        <v>27.410077455651834</v>
+        <v>43.28518335230283</v>
       </c>
       <c r="P8" s="0">
-        <v>56.2978047256697</v>
+        <v>118.33904970334234</v>
       </c>
       <c r="Q8" s="0">
-        <v>26.47196134009884</v>
+        <v>25.131773917755638</v>
       </c>
     </row>
     <row r="9">
@@ -576,54 +580,54 @@
         <v>4</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="D9" s="0">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E9" s="0">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F9" s="0">
-        <v>36.666666666666664</v>
+        <v>41</v>
       </c>
       <c r="G9" s="0">
-        <v>9.0615181460454579</v>
+        <v>12.335585379975555</v>
       </c>
       <c r="H9" s="0">
-        <v>8.3333333333333339</v>
+        <v>11</v>
       </c>
       <c r="I9" s="0">
-        <v>6.8879927732572757</v>
+        <v>5.7008771254956896</v>
       </c>
       <c r="J9" s="0">
-        <v>23.333333333333332</v>
+        <v>19.5</v>
       </c>
       <c r="K9" s="0">
-        <v>6.1734197258173786</v>
+        <v>6.0621778264910704</v>
       </c>
       <c r="L9" s="0">
-        <v>37.333333333333336</v>
+        <v>34.75</v>
       </c>
       <c r="M9" s="0">
-        <v>18.351506144667738</v>
+        <v>10.711170181948686</v>
       </c>
       <c r="N9" s="0">
-        <v>171.12352130325806</v>
+        <v>96.354627496159779</v>
       </c>
       <c r="O9" s="0">
-        <v>92.757489371524173</v>
+        <v>51.332148006698183</v>
       </c>
       <c r="P9" s="0">
-        <v>131.14162865217881</v>
+        <v>95.194464844370614</v>
       </c>
       <c r="Q9" s="0">
-        <v>31.421736740495735</v>
+        <v>31.337412702988139</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>4</v>
@@ -632,47 +636,51 @@
         <v>6</v>
       </c>
       <c r="D10" s="0">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E10" s="0">
         <v>4</v>
       </c>
       <c r="F10" s="0">
-        <v>19.25</v>
+        <v>22.5</v>
       </c>
       <c r="G10" s="0">
+        <v>10.267261887507626</v>
+      </c>
+      <c r="H10" s="0">
+        <v>2.75</v>
+      </c>
+      <c r="I10" s="0">
+        <v>1.4930394055974097</v>
+      </c>
+      <c r="J10" s="0">
+        <v>12.25</v>
+      </c>
+      <c r="K10" s="0">
         <v>6.2898728127045622</v>
       </c>
-      <c r="H10" s="0">
-        <v>8</v>
-      </c>
-      <c r="I10" s="0">
-        <v>2.6770630673681683</v>
-      </c>
-      <c r="J10" s="0">
-        <v>8.75</v>
-      </c>
-      <c r="K10" s="0">
-        <v>3.0923292192132452</v>
-      </c>
       <c r="L10" s="0">
-        <v>69</v>
+        <v>36.25</v>
       </c>
       <c r="M10" s="0">
-        <v>15.016657417681207</v>
-      </c>
-      <c r="N10" s="0"/>
-      <c r="O10" s="0"/>
+        <v>18.372874026673127</v>
+      </c>
+      <c r="N10" s="0">
+        <v>127.1013737060041</v>
+      </c>
+      <c r="O10" s="0">
+        <v>40.645243770063978</v>
+      </c>
       <c r="P10" s="0">
-        <v>0</v>
+        <v>61.021358264764288</v>
       </c>
       <c r="Q10" s="0">
-        <v>0</v>
+        <v>32.518021178612607</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>4</v>
@@ -681,51 +689,51 @@
         <v>6</v>
       </c>
       <c r="D11" s="0">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E11" s="0">
         <v>4</v>
       </c>
       <c r="F11" s="0">
-        <v>26.5</v>
+        <v>22.5</v>
       </c>
       <c r="G11" s="0">
-        <v>14.642973286415115</v>
+        <v>7.5</v>
       </c>
       <c r="H11" s="0">
-        <v>4.75</v>
+        <v>3.5</v>
       </c>
       <c r="I11" s="0">
-        <v>1.8874586088176875</v>
+        <v>0.6454972243679028</v>
       </c>
       <c r="J11" s="0">
-        <v>14.25</v>
+        <v>12.25</v>
       </c>
       <c r="K11" s="0">
-        <v>5.1700257897487001</v>
+        <v>4.3851073723076235</v>
       </c>
       <c r="L11" s="0">
-        <v>94</v>
+        <v>24.25</v>
       </c>
       <c r="M11" s="0">
-        <v>19.131126469708992</v>
+        <v>5.4217924465377072</v>
       </c>
       <c r="N11" s="0">
-        <v>22.168641025641094</v>
+        <v>222.01591666666653</v>
       </c>
       <c r="O11" s="0">
-        <v>10.533023318956069</v>
+        <v>193.05319351500069</v>
       </c>
       <c r="P11" s="0">
-        <v>49.994060601563049</v>
+        <v>60.442991085239044</v>
       </c>
       <c r="Q11" s="0">
-        <v>19.870402113019829</v>
+        <v>22.810139304691134</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>4</v>
@@ -734,104 +742,100 @@
         <v>6</v>
       </c>
       <c r="D12" s="0">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E12" s="0">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F12" s="0">
-        <v>31</v>
+        <v>26.5</v>
       </c>
       <c r="G12" s="0">
-        <v>10.583005244258363</v>
+        <v>5.634713834792322</v>
       </c>
       <c r="H12" s="0">
-        <v>8.3333333333333339</v>
+        <v>6.75</v>
       </c>
       <c r="I12" s="0">
-        <v>3.3333333333333335</v>
+        <v>2.809952550014561</v>
       </c>
       <c r="J12" s="0">
-        <v>15.333333333333334</v>
+        <v>15.5</v>
       </c>
       <c r="K12" s="0">
-        <v>4.0960685758148365</v>
+        <v>3.4034296427770228</v>
       </c>
       <c r="L12" s="0">
-        <v>50.666666666666664</v>
+        <v>32.5</v>
       </c>
       <c r="M12" s="0">
-        <v>6.6916199666282443</v>
+        <v>10.242883708539635</v>
       </c>
       <c r="N12" s="0">
-        <v>33.977886002886017</v>
+        <v>131.38006477732793</v>
       </c>
       <c r="O12" s="0">
-        <v>13.172894507551444</v>
+        <v>34.427451776658629</v>
       </c>
       <c r="P12" s="0">
-        <v>53.720718787482781</v>
+        <v>74.505491586046276</v>
       </c>
       <c r="Q12" s="0">
-        <v>16.626710579297754</v>
+        <v>16.548829800403684</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>4</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="D13" s="0">
+        <v>0</v>
+      </c>
+      <c r="E13" s="0">
         <v>3</v>
       </c>
-      <c r="E13" s="0">
-        <v>4</v>
-      </c>
       <c r="F13" s="0">
-        <v>52</v>
+        <v>22.333333333333332</v>
       </c>
       <c r="G13" s="0">
-        <v>13.90443574307614</v>
+        <v>5.8404718226450774</v>
       </c>
       <c r="H13" s="0">
-        <v>28</v>
+        <v>11.333333333333334</v>
       </c>
       <c r="I13" s="0">
-        <v>16.140012391568973</v>
+        <v>2.9059326290271157</v>
       </c>
       <c r="J13" s="0">
-        <v>32.75</v>
+        <v>11</v>
       </c>
       <c r="K13" s="0">
-        <v>7.7714756213561742</v>
+        <v>0.57735026918962584</v>
       </c>
       <c r="L13" s="0">
-        <v>85.25</v>
+        <v>42.666666666666664</v>
       </c>
       <c r="M13" s="0">
-        <v>17.899604278679831</v>
-      </c>
-      <c r="N13" s="0">
-        <v>65.366862207602395</v>
-      </c>
-      <c r="O13" s="0">
-        <v>32.454443000967174</v>
-      </c>
+        <v>13.245544324203685</v>
+      </c>
+      <c r="N13" s="0"/>
+      <c r="O13" s="0"/>
       <c r="P13" s="0">
-        <v>112.19959175674629</v>
+        <v>0</v>
       </c>
       <c r="Q13" s="0">
-        <v>27.388405886137765</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>4</v>
@@ -840,47 +844,51 @@
         <v>22</v>
       </c>
       <c r="D14" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" s="0">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F14" s="0">
-        <v>11.5</v>
+        <v>17.666666666666668</v>
       </c>
       <c r="G14" s="0">
-        <v>3.378855822118882</v>
+        <v>17.169093679567879</v>
       </c>
       <c r="H14" s="0">
-        <v>5.75</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="I14" s="0">
-        <v>1.1086778913041726</v>
+        <v>0.33333333333333337</v>
       </c>
       <c r="J14" s="0">
-        <v>6.75</v>
+        <v>11</v>
       </c>
       <c r="K14" s="0">
-        <v>1.973786547054502</v>
+        <v>10.503967504392488</v>
       </c>
       <c r="L14" s="0">
-        <v>26.75</v>
+        <v>66</v>
       </c>
       <c r="M14" s="0">
-        <v>2.5289984842489197</v>
-      </c>
-      <c r="N14" s="0"/>
-      <c r="O14" s="0"/>
+        <v>23.797758998135379</v>
+      </c>
+      <c r="N14" s="0">
+        <v>147.12807692307683</v>
+      </c>
+      <c r="O14" s="0">
+        <v>124.50807692307683</v>
+      </c>
       <c r="P14" s="0">
-        <v>0</v>
+        <v>59.720951008334417</v>
       </c>
       <c r="Q14" s="0">
-        <v>0</v>
+        <v>57.017462445790393</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>4</v>
@@ -889,49 +897,51 @@
         <v>22</v>
       </c>
       <c r="D15" s="0">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E15" s="0">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F15" s="0">
-        <v>29.75</v>
+        <v>15.666666666666666</v>
       </c>
       <c r="G15" s="0">
-        <v>12.51915199471061</v>
+        <v>7.4236858171066959</v>
       </c>
       <c r="H15" s="0">
-        <v>5.5</v>
+        <v>6.666666666666667</v>
       </c>
       <c r="I15" s="0">
-        <v>2.5331140255951108</v>
+        <v>6.666666666666667</v>
       </c>
       <c r="J15" s="0">
-        <v>18</v>
+        <v>9.6666666666666661</v>
       </c>
       <c r="K15" s="0">
-        <v>6.324555320336759</v>
+        <v>4.4845413490245702</v>
       </c>
       <c r="L15" s="0">
-        <v>49.75</v>
+        <v>62</v>
       </c>
       <c r="M15" s="0">
-        <v>11.678862672937521</v>
+        <v>15.176736583776281</v>
       </c>
       <c r="N15" s="0">
-        <v>199.02467307692302</v>
+        <v>50.378703703703508</v>
       </c>
       <c r="O15" s="0">
-        <v>83.158139318497049</v>
+        <v>27.410077455651834</v>
       </c>
       <c r="P15" s="0">
-        <v>65535</v>
-      </c>
-      <c r="Q15" s="0"/>
+        <v>56.2978047256697</v>
+      </c>
+      <c r="Q15" s="0">
+        <v>26.47196134009884</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="0" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>4</v>
@@ -940,51 +950,51 @@
         <v>22</v>
       </c>
       <c r="D16" s="0">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E16" s="0">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F16" s="0">
-        <v>28.5</v>
+        <v>36.666666666666664</v>
       </c>
       <c r="G16" s="0">
-        <v>8.4606934309980364</v>
+        <v>9.0615181460454579</v>
       </c>
       <c r="H16" s="0">
-        <v>4.5</v>
+        <v>8.3333333333333339</v>
       </c>
       <c r="I16" s="0">
-        <v>1.0408329997330663</v>
+        <v>6.8879927732572757</v>
       </c>
       <c r="J16" s="0">
-        <v>18.25</v>
+        <v>23.333333333333332</v>
       </c>
       <c r="K16" s="0">
-        <v>5.5283360968739954</v>
+        <v>6.1734197258173786</v>
       </c>
       <c r="L16" s="0">
-        <v>16.5</v>
+        <v>37.333333333333336</v>
       </c>
       <c r="M16" s="0">
-        <v>4.0926763859362252</v>
+        <v>18.351506144667738</v>
       </c>
       <c r="N16" s="0">
-        <v>123.76519444444445</v>
+        <v>171.12352130325806</v>
       </c>
       <c r="O16" s="0">
-        <v>96.563654110602727</v>
+        <v>92.757489371524173</v>
       </c>
       <c r="P16" s="0">
-        <v>57.096024507691922</v>
+        <v>131.14162865217881</v>
       </c>
       <c r="Q16" s="0">
-        <v>17.581199231611976</v>
+        <v>31.421736740495735</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>4</v>
@@ -993,45 +1003,1517 @@
         <v>22</v>
       </c>
       <c r="D17" s="0">
+        <v>4</v>
+      </c>
+      <c r="E17" s="0">
+        <v>4</v>
+      </c>
+      <c r="F17" s="0">
+        <v>49.75</v>
+      </c>
+      <c r="G17" s="0">
+        <v>32.208629795962032</v>
+      </c>
+      <c r="H17" s="0">
+        <v>3.25</v>
+      </c>
+      <c r="I17" s="0">
+        <v>2.6259918760981216</v>
+      </c>
+      <c r="J17" s="0">
+        <v>27.25</v>
+      </c>
+      <c r="K17" s="0">
+        <v>14.642261892663077</v>
+      </c>
+      <c r="L17" s="0">
+        <v>33</v>
+      </c>
+      <c r="M17" s="0">
+        <v>9.8064604555704342</v>
+      </c>
+      <c r="N17" s="0">
+        <v>194.54360256410257</v>
+      </c>
+      <c r="O17" s="0">
+        <v>47.180177760276493</v>
+      </c>
+      <c r="P17" s="0">
+        <v>151.34939789819879</v>
+      </c>
+      <c r="Q17" s="0">
+        <v>78.840681649188383</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="0">
+        <v>6</v>
+      </c>
+      <c r="E18" s="0">
         <v>3</v>
       </c>
-      <c r="E17" s="0">
-        <v>4</v>
-      </c>
-      <c r="F17" s="0">
+      <c r="F18" s="0">
+        <v>39.333333333333336</v>
+      </c>
+      <c r="G18" s="0">
+        <v>13.017082793177757</v>
+      </c>
+      <c r="H18" s="0">
+        <v>11.333333333333334</v>
+      </c>
+      <c r="I18" s="0">
+        <v>10.333333333333334</v>
+      </c>
+      <c r="J18" s="0">
+        <v>24.666666666666668</v>
+      </c>
+      <c r="K18" s="0">
+        <v>8.6666666666666679</v>
+      </c>
+      <c r="L18" s="0">
+        <v>38.666666666666664</v>
+      </c>
+      <c r="M18" s="0">
+        <v>1.2018504251546631</v>
+      </c>
+      <c r="N18" s="0">
+        <v>193.94226190476198</v>
+      </c>
+      <c r="O18" s="0">
+        <v>64.546990462261391</v>
+      </c>
+      <c r="P18" s="0">
+        <v>135.36147039755053</v>
+      </c>
+      <c r="Q18" s="0">
+        <v>47.607984224371108</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="0">
+        <v>7</v>
+      </c>
+      <c r="E19" s="0">
+        <v>3</v>
+      </c>
+      <c r="F19" s="0">
+        <v>20.666666666666668</v>
+      </c>
+      <c r="G19" s="0">
+        <v>7.2188026092359054</v>
+      </c>
+      <c r="H19" s="0">
+        <v>2.3333333333333335</v>
+      </c>
+      <c r="I19" s="0">
+        <v>1.8559214542766742</v>
+      </c>
+      <c r="J19" s="0">
+        <v>16</v>
+      </c>
+      <c r="K19" s="0">
+        <v>3.2145502536643185</v>
+      </c>
+      <c r="L19" s="0">
+        <v>28.333333333333332</v>
+      </c>
+      <c r="M19" s="0">
+        <v>15.719768163402129</v>
+      </c>
+      <c r="N19" s="0">
+        <v>141.20233333333331</v>
+      </c>
+      <c r="O19" s="0">
+        <v>26.809651749433957</v>
+      </c>
+      <c r="P19" s="0">
+        <v>89.13695704326004</v>
+      </c>
+      <c r="Q19" s="0">
+        <v>19.774548598661202</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="0">
+        <v>8</v>
+      </c>
+      <c r="E20" s="0">
+        <v>3</v>
+      </c>
+      <c r="F20" s="0">
+        <v>26.666666666666668</v>
+      </c>
+      <c r="G20" s="0">
+        <v>9.9554563487120529</v>
+      </c>
+      <c r="H20" s="0">
+        <v>4.666666666666667</v>
+      </c>
+      <c r="I20" s="0">
+        <v>4.1766546953805559</v>
+      </c>
+      <c r="J20" s="0">
+        <v>19.333333333333332</v>
+      </c>
+      <c r="K20" s="0">
+        <v>5.7831171909658243</v>
+      </c>
+      <c r="L20" s="0">
+        <v>34.666666666666664</v>
+      </c>
+      <c r="M20" s="0">
+        <v>11.89304184994085</v>
+      </c>
+      <c r="N20" s="0">
+        <v>103.55441798941801</v>
+      </c>
+      <c r="O20" s="0">
+        <v>31.842857207617705</v>
+      </c>
+      <c r="P20" s="0">
+        <v>108.15475427996523</v>
+      </c>
+      <c r="Q20" s="0">
+        <v>33.800915352693998</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" s="0">
+        <v>9</v>
+      </c>
+      <c r="E21" s="0">
+        <v>3</v>
+      </c>
+      <c r="F21" s="0">
+        <v>14.666666666666666</v>
+      </c>
+      <c r="G21" s="0">
+        <v>2.728450923957483</v>
+      </c>
+      <c r="H21" s="0">
+        <v>6.333333333333333</v>
+      </c>
+      <c r="I21" s="0">
+        <v>3.2829526005987018</v>
+      </c>
+      <c r="J21" s="0">
+        <v>12.333333333333334</v>
+      </c>
+      <c r="K21" s="0">
+        <v>2.8480012484391777</v>
+      </c>
+      <c r="L21" s="0">
+        <v>24.333333333333332</v>
+      </c>
+      <c r="M21" s="0">
+        <v>9.4044906531105923</v>
+      </c>
+      <c r="N21" s="0">
+        <v>259.80317460317463</v>
+      </c>
+      <c r="O21" s="0">
+        <v>181.81741983243114</v>
+      </c>
+      <c r="P21" s="0">
+        <v>67.453179995532537</v>
+      </c>
+      <c r="Q21" s="0">
+        <v>14.024567676957011</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" s="0">
+        <v>10</v>
+      </c>
+      <c r="E22" s="0">
+        <v>3</v>
+      </c>
+      <c r="F22" s="0">
+        <v>10.333333333333334</v>
+      </c>
+      <c r="G22" s="0">
+        <v>2.3333333333333335</v>
+      </c>
+      <c r="H22" s="0">
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="I22" s="0">
+        <v>0.88191710368819698</v>
+      </c>
+      <c r="J22" s="0">
+        <v>9</v>
+      </c>
+      <c r="K22" s="0">
+        <v>1</v>
+      </c>
+      <c r="L22" s="0">
+        <v>35.333333333333336</v>
+      </c>
+      <c r="M22" s="0">
+        <v>14.847371634213394</v>
+      </c>
+      <c r="N22" s="0">
+        <v>187.92211640211642</v>
+      </c>
+      <c r="O22" s="0">
+        <v>107.7609416840225</v>
+      </c>
+      <c r="P22" s="0">
+        <v>49.909091132794707</v>
+      </c>
+      <c r="Q22" s="0">
+        <v>6.5701566750317086</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" s="0">
+        <v>11</v>
+      </c>
+      <c r="E23" s="0">
+        <v>3</v>
+      </c>
+      <c r="F23" s="0">
+        <v>54.333333333333336</v>
+      </c>
+      <c r="G23" s="0">
+        <v>5.0442486501405197</v>
+      </c>
+      <c r="H23" s="0">
+        <v>7.666666666666667</v>
+      </c>
+      <c r="I23" s="0">
+        <v>3.2829526005987018</v>
+      </c>
+      <c r="J23" s="0">
+        <v>38.333333333333336</v>
+      </c>
+      <c r="K23" s="0">
+        <v>3.8441875315569325</v>
+      </c>
+      <c r="L23" s="0">
+        <v>40.333333333333336</v>
+      </c>
+      <c r="M23" s="0">
+        <v>16.333333333333332</v>
+      </c>
+      <c r="N23" s="0">
+        <v>242.66604797979792</v>
+      </c>
+      <c r="O23" s="0">
+        <v>85.094911956049671</v>
+      </c>
+      <c r="P23" s="0">
+        <v>208.23127448771447</v>
+      </c>
+      <c r="Q23" s="0">
+        <v>23.504791614783297</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="0">
+        <v>0</v>
+      </c>
+      <c r="E24" s="0">
+        <v>4</v>
+      </c>
+      <c r="F24" s="0">
+        <v>19.25</v>
+      </c>
+      <c r="G24" s="0">
+        <v>6.2898728127045622</v>
+      </c>
+      <c r="H24" s="0">
+        <v>8</v>
+      </c>
+      <c r="I24" s="0">
+        <v>2.6770630673681683</v>
+      </c>
+      <c r="J24" s="0">
+        <v>8.75</v>
+      </c>
+      <c r="K24" s="0">
+        <v>3.0923292192132452</v>
+      </c>
+      <c r="L24" s="0">
+        <v>69</v>
+      </c>
+      <c r="M24" s="0">
+        <v>15.016657417681207</v>
+      </c>
+      <c r="N24" s="0"/>
+      <c r="O24" s="0"/>
+      <c r="P24" s="0">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="0">
+        <v>1</v>
+      </c>
+      <c r="E25" s="0">
+        <v>4</v>
+      </c>
+      <c r="F25" s="0">
+        <v>26.5</v>
+      </c>
+      <c r="G25" s="0">
+        <v>14.642973286415115</v>
+      </c>
+      <c r="H25" s="0">
+        <v>4.75</v>
+      </c>
+      <c r="I25" s="0">
+        <v>1.8874586088176875</v>
+      </c>
+      <c r="J25" s="0">
+        <v>14.25</v>
+      </c>
+      <c r="K25" s="0">
+        <v>5.1700257897487001</v>
+      </c>
+      <c r="L25" s="0">
+        <v>94</v>
+      </c>
+      <c r="M25" s="0">
+        <v>19.131126469708992</v>
+      </c>
+      <c r="N25" s="0">
+        <v>22.168641025641094</v>
+      </c>
+      <c r="O25" s="0">
+        <v>10.533023318956069</v>
+      </c>
+      <c r="P25" s="0">
+        <v>49.994060601563049</v>
+      </c>
+      <c r="Q25" s="0">
+        <v>19.870402113019829</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="0">
+        <v>2</v>
+      </c>
+      <c r="E26" s="0">
+        <v>3</v>
+      </c>
+      <c r="F26" s="0">
+        <v>31</v>
+      </c>
+      <c r="G26" s="0">
+        <v>10.583005244258363</v>
+      </c>
+      <c r="H26" s="0">
+        <v>8.3333333333333339</v>
+      </c>
+      <c r="I26" s="0">
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="J26" s="0">
+        <v>15.333333333333334</v>
+      </c>
+      <c r="K26" s="0">
+        <v>4.0960685758148365</v>
+      </c>
+      <c r="L26" s="0">
+        <v>50.666666666666664</v>
+      </c>
+      <c r="M26" s="0">
+        <v>6.6916199666282443</v>
+      </c>
+      <c r="N26" s="0">
+        <v>33.977886002886017</v>
+      </c>
+      <c r="O26" s="0">
+        <v>13.172894507551444</v>
+      </c>
+      <c r="P26" s="0">
+        <v>53.720718787482781</v>
+      </c>
+      <c r="Q26" s="0">
+        <v>16.626710579297754</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" s="0">
+        <v>3</v>
+      </c>
+      <c r="E27" s="0">
+        <v>4</v>
+      </c>
+      <c r="F27" s="0">
+        <v>52</v>
+      </c>
+      <c r="G27" s="0">
+        <v>13.90443574307614</v>
+      </c>
+      <c r="H27" s="0">
+        <v>28</v>
+      </c>
+      <c r="I27" s="0">
+        <v>16.140012391568973</v>
+      </c>
+      <c r="J27" s="0">
+        <v>32.75</v>
+      </c>
+      <c r="K27" s="0">
+        <v>7.7714756213561742</v>
+      </c>
+      <c r="L27" s="0">
+        <v>85.25</v>
+      </c>
+      <c r="M27" s="0">
+        <v>17.899604278679831</v>
+      </c>
+      <c r="N27" s="0">
+        <v>65.366862207602395</v>
+      </c>
+      <c r="O27" s="0">
+        <v>32.454443000967174</v>
+      </c>
+      <c r="P27" s="0">
+        <v>112.19959175674629</v>
+      </c>
+      <c r="Q27" s="0">
+        <v>27.388405886137765</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" s="0">
+        <v>4</v>
+      </c>
+      <c r="E28" s="0">
+        <v>6</v>
+      </c>
+      <c r="F28" s="0">
+        <v>34.5</v>
+      </c>
+      <c r="G28" s="0">
+        <v>7.9529868602934339</v>
+      </c>
+      <c r="H28" s="0">
+        <v>10.666666666666666</v>
+      </c>
+      <c r="I28" s="0">
+        <v>3.2214558475598856</v>
+      </c>
+      <c r="J28" s="0">
+        <v>23.833333333333332</v>
+      </c>
+      <c r="K28" s="0">
+        <v>6.4777396606463817</v>
+      </c>
+      <c r="L28" s="0">
+        <v>49.666666666666664</v>
+      </c>
+      <c r="M28" s="0">
+        <v>6.6916199666282434</v>
+      </c>
+      <c r="N28" s="0">
+        <v>87.773193392255891</v>
+      </c>
+      <c r="O28" s="0">
+        <v>37.660379526578986</v>
+      </c>
+      <c r="P28" s="0">
+        <v>78.719213084333219</v>
+      </c>
+      <c r="Q28" s="0">
+        <v>20.497351046408252</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" s="0">
+        <v>6</v>
+      </c>
+      <c r="E29" s="0">
+        <v>4</v>
+      </c>
+      <c r="F29" s="0">
+        <v>24.5</v>
+      </c>
+      <c r="G29" s="0">
+        <v>4.7346242371139304</v>
+      </c>
+      <c r="H29" s="0">
+        <v>9.25</v>
+      </c>
+      <c r="I29" s="0">
+        <v>1.7017148213885114</v>
+      </c>
+      <c r="J29" s="0">
+        <v>20.25</v>
+      </c>
+      <c r="K29" s="0">
+        <v>3.2242570203588508</v>
+      </c>
+      <c r="L29" s="0">
+        <v>43.75</v>
+      </c>
+      <c r="M29" s="0">
+        <v>11.685995892520243</v>
+      </c>
+      <c r="N29" s="0">
+        <v>58.356144480519482</v>
+      </c>
+      <c r="O29" s="0">
+        <v>39.025444277436456</v>
+      </c>
+      <c r="P29" s="0">
+        <v>66.345643537008328</v>
+      </c>
+      <c r="Q29" s="0">
+        <v>10.408746001378843</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="0">
+        <v>7</v>
+      </c>
+      <c r="E30" s="0">
+        <v>4</v>
+      </c>
+      <c r="F30" s="0">
+        <v>24.75</v>
+      </c>
+      <c r="G30" s="0">
+        <v>5.5883062430996624</v>
+      </c>
+      <c r="H30" s="0">
+        <v>12.5</v>
+      </c>
+      <c r="I30" s="0">
+        <v>1.8929694486000912</v>
+      </c>
+      <c r="J30" s="0">
+        <v>19.5</v>
+      </c>
+      <c r="K30" s="0">
+        <v>4.2914643965279113</v>
+      </c>
+      <c r="L30" s="0">
+        <v>42.5</v>
+      </c>
+      <c r="M30" s="0">
+        <v>5.634713834792322</v>
+      </c>
+      <c r="N30" s="0">
+        <v>98.323651789386957</v>
+      </c>
+      <c r="O30" s="0">
+        <v>43.959531955662413</v>
+      </c>
+      <c r="P30" s="0">
+        <v>64.777571457735448</v>
+      </c>
+      <c r="Q30" s="0">
+        <v>15.103410376999443</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" s="0">
+        <v>8</v>
+      </c>
+      <c r="E31" s="0">
+        <v>4</v>
+      </c>
+      <c r="F31" s="0">
+        <v>22.75</v>
+      </c>
+      <c r="G31" s="0">
+        <v>3.6827299656640586</v>
+      </c>
+      <c r="H31" s="0">
+        <v>8.75</v>
+      </c>
+      <c r="I31" s="0">
+        <v>2.6887109674836132</v>
+      </c>
+      <c r="J31" s="0">
+        <v>15.25</v>
+      </c>
+      <c r="K31" s="0">
+        <v>2.2126530078919591</v>
+      </c>
+      <c r="L31" s="0">
+        <v>47</v>
+      </c>
+      <c r="M31" s="0">
+        <v>12.935738607954837</v>
+      </c>
+      <c r="N31" s="0">
+        <v>157.92080176767675</v>
+      </c>
+      <c r="O31" s="0">
+        <v>83.227737171056702</v>
+      </c>
+      <c r="P31" s="0">
+        <v>50.256551304898892</v>
+      </c>
+      <c r="Q31" s="0">
+        <v>7.7511695070748141</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="0">
+        <v>9</v>
+      </c>
+      <c r="E32" s="0">
+        <v>4</v>
+      </c>
+      <c r="F32" s="0">
+        <v>29.5</v>
+      </c>
+      <c r="G32" s="0">
+        <v>4.1733280085163047</v>
+      </c>
+      <c r="H32" s="0">
+        <v>5.75</v>
+      </c>
+      <c r="I32" s="0">
+        <v>1.4930394055974097</v>
+      </c>
+      <c r="J32" s="0">
+        <v>19.75</v>
+      </c>
+      <c r="K32" s="0">
+        <v>2.2867371223353739</v>
+      </c>
+      <c r="L32" s="0">
+        <v>50.75</v>
+      </c>
+      <c r="M32" s="0">
+        <v>16.131620088096131</v>
+      </c>
+      <c r="N32" s="0">
+        <v>65.46980357142867</v>
+      </c>
+      <c r="O32" s="0">
+        <v>42.191087062516566</v>
+      </c>
+      <c r="P32" s="0">
+        <v>64.147899335807864</v>
+      </c>
+      <c r="Q32" s="0">
+        <v>5.9704849097917378</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" s="0">
+        <v>10</v>
+      </c>
+      <c r="E33" s="0">
+        <v>4</v>
+      </c>
+      <c r="F33" s="0">
+        <v>26.25</v>
+      </c>
+      <c r="G33" s="0">
+        <v>6.3688696014284982</v>
+      </c>
+      <c r="H33" s="0">
+        <v>5</v>
+      </c>
+      <c r="I33" s="0">
+        <v>1.2909944487358056</v>
+      </c>
+      <c r="J33" s="0">
+        <v>19.5</v>
+      </c>
+      <c r="K33" s="0">
+        <v>4.4253060157839181</v>
+      </c>
+      <c r="L33" s="0">
+        <v>52.25</v>
+      </c>
+      <c r="M33" s="0">
+        <v>7.3979163733220625</v>
+      </c>
+      <c r="N33" s="0">
+        <v>76.725373376623381</v>
+      </c>
+      <c r="O33" s="0">
+        <v>69.106430857045268</v>
+      </c>
+      <c r="P33" s="0">
+        <v>63.31241883365562</v>
+      </c>
+      <c r="Q33" s="0">
+        <v>13.870452293565409</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" s="0">
+        <v>11</v>
+      </c>
+      <c r="E34" s="0">
+        <v>4</v>
+      </c>
+      <c r="F34" s="0">
+        <v>25.75</v>
+      </c>
+      <c r="G34" s="0">
+        <v>3.966001344763598</v>
+      </c>
+      <c r="H34" s="0">
+        <v>4.5</v>
+      </c>
+      <c r="I34" s="0">
+        <v>1.9364916731037085</v>
+      </c>
+      <c r="J34" s="0">
+        <v>20.25</v>
+      </c>
+      <c r="K34" s="0">
+        <v>2.0155644370746373</v>
+      </c>
+      <c r="L34" s="0">
+        <v>48.25</v>
+      </c>
+      <c r="M34" s="0">
+        <v>11.360567767501763</v>
+      </c>
+      <c r="N34" s="0">
+        <v>51.138666666666744</v>
+      </c>
+      <c r="O34" s="0">
+        <v>40.114655891304643</v>
+      </c>
+      <c r="P34" s="0">
+        <v>64.238335695371177</v>
+      </c>
+      <c r="Q34" s="0">
+        <v>4.4645526493660395</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D35" s="0">
+        <v>0</v>
+      </c>
+      <c r="E35" s="0">
+        <v>4</v>
+      </c>
+      <c r="F35" s="0">
+        <v>11.5</v>
+      </c>
+      <c r="G35" s="0">
+        <v>3.378855822118882</v>
+      </c>
+      <c r="H35" s="0">
+        <v>5.75</v>
+      </c>
+      <c r="I35" s="0">
+        <v>1.1086778913041726</v>
+      </c>
+      <c r="J35" s="0">
+        <v>6.75</v>
+      </c>
+      <c r="K35" s="0">
+        <v>1.973786547054502</v>
+      </c>
+      <c r="L35" s="0">
+        <v>26.75</v>
+      </c>
+      <c r="M35" s="0">
+        <v>2.5289984842489197</v>
+      </c>
+      <c r="N35" s="0"/>
+      <c r="O35" s="0"/>
+      <c r="P35" s="0">
+        <v>0</v>
+      </c>
+      <c r="Q35" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D36" s="0">
+        <v>1</v>
+      </c>
+      <c r="E36" s="0">
+        <v>4</v>
+      </c>
+      <c r="F36" s="0">
+        <v>29.75</v>
+      </c>
+      <c r="G36" s="0">
+        <v>12.51915199471061</v>
+      </c>
+      <c r="H36" s="0">
+        <v>5.5</v>
+      </c>
+      <c r="I36" s="0">
+        <v>2.5331140255951108</v>
+      </c>
+      <c r="J36" s="0">
+        <v>18</v>
+      </c>
+      <c r="K36" s="0">
+        <v>6.324555320336759</v>
+      </c>
+      <c r="L36" s="0">
+        <v>49.75</v>
+      </c>
+      <c r="M36" s="0">
+        <v>11.678862672937521</v>
+      </c>
+      <c r="N36" s="0">
+        <v>199.02467307692302</v>
+      </c>
+      <c r="O36" s="0">
+        <v>83.158139318497049</v>
+      </c>
+      <c r="P36" s="0">
+        <v>65535</v>
+      </c>
+      <c r="Q36" s="0"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D37" s="0">
+        <v>2</v>
+      </c>
+      <c r="E37" s="0">
+        <v>4</v>
+      </c>
+      <c r="F37" s="0">
+        <v>28.5</v>
+      </c>
+      <c r="G37" s="0">
+        <v>8.4606934309980364</v>
+      </c>
+      <c r="H37" s="0">
+        <v>4.5</v>
+      </c>
+      <c r="I37" s="0">
+        <v>1.0408329997330663</v>
+      </c>
+      <c r="J37" s="0">
+        <v>18.25</v>
+      </c>
+      <c r="K37" s="0">
+        <v>5.5283360968739954</v>
+      </c>
+      <c r="L37" s="0">
+        <v>16.5</v>
+      </c>
+      <c r="M37" s="0">
+        <v>4.0926763859362252</v>
+      </c>
+      <c r="N37" s="0">
+        <v>123.76519444444445</v>
+      </c>
+      <c r="O37" s="0">
+        <v>96.563654110602727</v>
+      </c>
+      <c r="P37" s="0">
+        <v>57.096024507691922</v>
+      </c>
+      <c r="Q37" s="0">
+        <v>17.581199231611976</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D38" s="0">
+        <v>3</v>
+      </c>
+      <c r="E38" s="0">
+        <v>4</v>
+      </c>
+      <c r="F38" s="0">
         <v>54.25</v>
       </c>
-      <c r="G17" s="0">
+      <c r="G38" s="0">
         <v>23.264332499916403</v>
       </c>
-      <c r="H17" s="0">
+      <c r="H38" s="0">
         <v>12</v>
       </c>
-      <c r="I17" s="0">
+      <c r="I38" s="0">
         <v>5.8166427888717163</v>
       </c>
-      <c r="J17" s="0">
+      <c r="J38" s="0">
         <v>37</v>
       </c>
-      <c r="K17" s="0">
+      <c r="K38" s="0">
         <v>16.416455159382004</v>
       </c>
-      <c r="L17" s="0">
+      <c r="L38" s="0">
         <v>29.25</v>
       </c>
-      <c r="M17" s="0">
+      <c r="M38" s="0">
         <v>7.1922991224410753</v>
       </c>
-      <c r="N17" s="0">
+      <c r="N38" s="0">
         <v>396.74887121212117</v>
       </c>
-      <c r="O17" s="0">
+      <c r="O38" s="0">
         <v>320.97552634128039</v>
       </c>
-      <c r="P17" s="0">
+      <c r="P38" s="0">
         <v>65535</v>
       </c>
-      <c r="Q17" s="0"/>
+      <c r="Q38" s="0"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D39" s="0">
+        <v>4</v>
+      </c>
+      <c r="E39" s="0">
+        <v>6</v>
+      </c>
+      <c r="F39" s="0">
+        <v>41.666666666666664</v>
+      </c>
+      <c r="G39" s="0">
+        <v>15.730366951995888</v>
+      </c>
+      <c r="H39" s="0">
+        <v>5.166666666666667</v>
+      </c>
+      <c r="I39" s="0">
+        <v>1.7779513804126119</v>
+      </c>
+      <c r="J39" s="0">
+        <v>33.333333333333336</v>
+      </c>
+      <c r="K39" s="0">
+        <v>11.757739767678329</v>
+      </c>
+      <c r="L39" s="0">
+        <v>21.333333333333332</v>
+      </c>
+      <c r="M39" s="0">
+        <v>5.9142013643245006</v>
+      </c>
+      <c r="N39" s="0">
+        <v>285.32431818181823</v>
+      </c>
+      <c r="O39" s="0">
+        <v>180.48152809142471</v>
+      </c>
+      <c r="P39" s="0">
+        <v>103.3947270594149</v>
+      </c>
+      <c r="Q39" s="0">
+        <v>35.958230595396941</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D40" s="0">
+        <v>6</v>
+      </c>
+      <c r="E40" s="0">
+        <v>4</v>
+      </c>
+      <c r="F40" s="0">
+        <v>26</v>
+      </c>
+      <c r="G40" s="0">
+        <v>9.9582461641931044</v>
+      </c>
+      <c r="H40" s="0">
+        <v>6.75</v>
+      </c>
+      <c r="I40" s="0">
+        <v>2.6575364531836625</v>
+      </c>
+      <c r="J40" s="0">
+        <v>20.75</v>
+      </c>
+      <c r="K40" s="0">
+        <v>8.1687922403906601</v>
+      </c>
+      <c r="L40" s="0">
+        <v>22.5</v>
+      </c>
+      <c r="M40" s="0">
+        <v>4.1932485418030412</v>
+      </c>
+      <c r="N40" s="0">
+        <v>347.29934920634918</v>
+      </c>
+      <c r="O40" s="0">
+        <v>158.54349546179873</v>
+      </c>
+      <c r="P40" s="0">
+        <v>65535</v>
+      </c>
+      <c r="Q40" s="0"/>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D41" s="0">
+        <v>7</v>
+      </c>
+      <c r="E41" s="0">
+        <v>4</v>
+      </c>
+      <c r="F41" s="0">
+        <v>22.75</v>
+      </c>
+      <c r="G41" s="0">
+        <v>7.9621500446382782</v>
+      </c>
+      <c r="H41" s="0">
+        <v>3.75</v>
+      </c>
+      <c r="I41" s="0">
+        <v>1.6520189667999174</v>
+      </c>
+      <c r="J41" s="0">
+        <v>20.25</v>
+      </c>
+      <c r="K41" s="0">
+        <v>7.2154348448309058</v>
+      </c>
+      <c r="L41" s="0">
+        <v>22.75</v>
+      </c>
+      <c r="M41" s="0">
+        <v>7.9201746613737418</v>
+      </c>
+      <c r="N41" s="0">
+        <v>708.12724358974367</v>
+      </c>
+      <c r="O41" s="0">
+        <v>561.21766446431354</v>
+      </c>
+      <c r="P41" s="0">
+        <v>59.918759272660409</v>
+      </c>
+      <c r="Q41" s="0">
+        <v>21.035766353192841</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D42" s="0">
+        <v>8</v>
+      </c>
+      <c r="E42" s="0">
+        <v>4</v>
+      </c>
+      <c r="F42" s="0">
+        <v>33.25</v>
+      </c>
+      <c r="G42" s="0">
+        <v>5.1051444641655346</v>
+      </c>
+      <c r="H42" s="0">
+        <v>7.5</v>
+      </c>
+      <c r="I42" s="0">
+        <v>2.5331140255951108</v>
+      </c>
+      <c r="J42" s="0">
+        <v>25.75</v>
+      </c>
+      <c r="K42" s="0">
+        <v>3.6371921404658658</v>
+      </c>
+      <c r="L42" s="0">
+        <v>24.25</v>
+      </c>
+      <c r="M42" s="0">
+        <v>4.7147817199385456</v>
+      </c>
+      <c r="N42" s="0">
+        <v>142.98126893939397</v>
+      </c>
+      <c r="O42" s="0">
+        <v>36.959966323550475</v>
+      </c>
+      <c r="P42" s="0">
+        <v>75.952174842019758</v>
+      </c>
+      <c r="Q42" s="0">
+        <v>10.026028158088602</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D43" s="0">
+        <v>9</v>
+      </c>
+      <c r="E43" s="0">
+        <v>4</v>
+      </c>
+      <c r="F43" s="0">
+        <v>17.25</v>
+      </c>
+      <c r="G43" s="0">
+        <v>4.732423621500228</v>
+      </c>
+      <c r="H43" s="0">
+        <v>9.25</v>
+      </c>
+      <c r="I43" s="0">
+        <v>6.9686799323831767</v>
+      </c>
+      <c r="J43" s="0">
+        <v>14.25</v>
+      </c>
+      <c r="K43" s="0">
+        <v>4.4040700872412701</v>
+      </c>
+      <c r="L43" s="0">
+        <v>31</v>
+      </c>
+      <c r="M43" s="0">
+        <v>18.605554726120548</v>
+      </c>
+      <c r="N43" s="0">
+        <v>306.30527777777775</v>
+      </c>
+      <c r="O43" s="0">
+        <v>144.64282161794904</v>
+      </c>
+      <c r="P43" s="0">
+        <v>42.255216679264713</v>
+      </c>
+      <c r="Q43" s="0">
+        <v>13.15467278835462</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D44" s="0">
+        <v>10</v>
+      </c>
+      <c r="E44" s="0">
+        <v>4</v>
+      </c>
+      <c r="F44" s="0">
+        <v>16.25</v>
+      </c>
+      <c r="G44" s="0">
+        <v>5.5733742024019888</v>
+      </c>
+      <c r="H44" s="0">
+        <v>1</v>
+      </c>
+      <c r="I44" s="0">
+        <v>0.57735026918962573</v>
+      </c>
+      <c r="J44" s="0">
+        <v>11.25</v>
+      </c>
+      <c r="K44" s="0">
+        <v>3.7052890125692848</v>
+      </c>
+      <c r="L44" s="0">
+        <v>19</v>
+      </c>
+      <c r="M44" s="0">
+        <v>3.7638632635454048</v>
+      </c>
+      <c r="N44" s="0">
+        <v>180.63086507936512</v>
+      </c>
+      <c r="O44" s="0">
+        <v>56.827780897825768</v>
+      </c>
+      <c r="P44" s="0">
+        <v>33.331271553867516</v>
+      </c>
+      <c r="Q44" s="0">
+        <v>10.908418051016014</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D45" s="0">
+        <v>11</v>
+      </c>
+      <c r="E45" s="0">
+        <v>4</v>
+      </c>
+      <c r="F45" s="0">
+        <v>20.25</v>
+      </c>
+      <c r="G45" s="0">
+        <v>4.3851073723076235</v>
+      </c>
+      <c r="H45" s="0">
+        <v>6.25</v>
+      </c>
+      <c r="I45" s="0">
+        <v>0.8539125638299665</v>
+      </c>
+      <c r="J45" s="0">
+        <v>14.75</v>
+      </c>
+      <c r="K45" s="0">
+        <v>3.4247870980057527</v>
+      </c>
+      <c r="L45" s="0">
+        <v>28.25</v>
+      </c>
+      <c r="M45" s="0">
+        <v>3.2755406678389241</v>
+      </c>
+      <c r="N45" s="0">
+        <v>37.815684210526243</v>
+      </c>
+      <c r="O45" s="0">
+        <v>1.8994763552843577</v>
+      </c>
+      <c r="P45" s="0">
+        <v>42.611982644485956</v>
+      </c>
+      <c r="Q45" s="0">
+        <v>9.8438187406455917</v>
+      </c>
     </row>
   </sheetData>
 </worksheet>

</xml_diff>

<commit_message>
data 4/10-11 added, mild fixes
a few edits to checkSessionData.m and createMasterTable.m to make them function with the rat code.
</commit_message>
<xml_diff>
--- a/All Outputs/Exp_all_Run_all_exclusions/Behavior Tables/run_all_exp_ER_GroupStats.xlsx
+++ b/All Outputs/Exp_all_Run_all_exclusions/Behavior Tables/run_all_exp_ER_GroupStats.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="407" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="616" uniqueCount="23">
   <si>
     <t>Sex</t>
   </si>
@@ -127,7 +127,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q45"/>
+  <dimension ref="A1:Q65"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -427,43 +427,43 @@
         <v>4</v>
       </c>
       <c r="E6" s="0">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F6" s="0">
-        <v>92.166666666666671</v>
+        <v>79.5</v>
       </c>
       <c r="G6" s="0">
-        <v>38.300058021423993</v>
+        <v>41.48995862454754</v>
       </c>
       <c r="H6" s="0">
-        <v>11</v>
+        <v>15.25</v>
       </c>
       <c r="I6" s="0">
-        <v>5.3789714010518157</v>
+        <v>7.3640455367051247</v>
       </c>
       <c r="J6" s="0">
-        <v>39.5</v>
+        <v>36.75</v>
       </c>
       <c r="K6" s="0">
-        <v>15.411575736006577</v>
+        <v>19.241340043423865</v>
       </c>
       <c r="L6" s="0">
-        <v>83.333333333333329</v>
+        <v>82</v>
       </c>
       <c r="M6" s="0">
-        <v>32.352915032669173</v>
+        <v>40.648903224236363</v>
       </c>
       <c r="N6" s="0">
-        <v>161.37142538471747</v>
+        <v>88.753502274607158</v>
       </c>
       <c r="O6" s="0">
-        <v>103.62554349065974</v>
+        <v>77.570320102848825</v>
       </c>
       <c r="P6" s="0">
-        <v>216.24832893199013</v>
+        <v>197.80043177866068</v>
       </c>
       <c r="Q6" s="0">
-        <v>89.529740512532555</v>
+        <v>112.0929134675757</v>
       </c>
     </row>
     <row r="7">
@@ -477,46 +477,46 @@
         <v>6</v>
       </c>
       <c r="D7" s="0">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E7" s="0">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F7" s="0">
-        <v>32.75</v>
+        <v>117.5</v>
       </c>
       <c r="G7" s="0">
-        <v>14.378079380315949</v>
+        <v>103.49999999999999</v>
       </c>
       <c r="H7" s="0">
-        <v>5.25</v>
+        <v>2.5</v>
       </c>
       <c r="I7" s="0">
-        <v>2.8686524130097508</v>
+        <v>0.5</v>
       </c>
       <c r="J7" s="0">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="K7" s="0">
-        <v>6.1237243569579451</v>
+        <v>36</v>
       </c>
       <c r="L7" s="0">
-        <v>36.5</v>
+        <v>86</v>
       </c>
       <c r="M7" s="0">
-        <v>16.132265804901678</v>
+        <v>76</v>
       </c>
       <c r="N7" s="0">
-        <v>257.74884313725494</v>
+        <v>306.60727160493815</v>
       </c>
       <c r="O7" s="0">
-        <v>162.82175183132367</v>
+        <v>305.50072839506157</v>
       </c>
       <c r="P7" s="0">
-        <v>83.270458655521409</v>
+        <v>253.14412323864909</v>
       </c>
       <c r="Q7" s="0">
-        <v>30.552435766713579</v>
+        <v>206.88822970252741</v>
       </c>
     </row>
     <row r="8">
@@ -530,46 +530,46 @@
         <v>6</v>
       </c>
       <c r="D8" s="0">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E8" s="0">
         <v>4</v>
       </c>
       <c r="F8" s="0">
-        <v>46.5</v>
+        <v>32.75</v>
       </c>
       <c r="G8" s="0">
-        <v>11.84271928232701</v>
+        <v>14.378079380315949</v>
       </c>
       <c r="H8" s="0">
+        <v>5.25</v>
+      </c>
+      <c r="I8" s="0">
+        <v>2.8686524130097508</v>
+      </c>
+      <c r="J8" s="0">
         <v>17</v>
       </c>
-      <c r="I8" s="0">
-        <v>5.1153364177409353</v>
-      </c>
-      <c r="J8" s="0">
-        <v>24.25</v>
-      </c>
       <c r="K8" s="0">
-        <v>5.1861192941672032</v>
+        <v>6.1237243569579451</v>
       </c>
       <c r="L8" s="0">
-        <v>32</v>
+        <v>36.5</v>
       </c>
       <c r="M8" s="0">
-        <v>7.2915476180757857</v>
+        <v>16.132265804901678</v>
       </c>
       <c r="N8" s="0">
-        <v>117.15584108946607</v>
+        <v>257.74884313725494</v>
       </c>
       <c r="O8" s="0">
-        <v>43.28518335230283</v>
+        <v>162.82175183132367</v>
       </c>
       <c r="P8" s="0">
-        <v>118.33904970334234</v>
+        <v>83.270458655521409</v>
       </c>
       <c r="Q8" s="0">
-        <v>25.131773917755638</v>
+        <v>30.552435766713579</v>
       </c>
     </row>
     <row r="9">
@@ -583,46 +583,46 @@
         <v>6</v>
       </c>
       <c r="D9" s="0">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E9" s="0">
         <v>4</v>
       </c>
       <c r="F9" s="0">
-        <v>41</v>
+        <v>46.5</v>
       </c>
       <c r="G9" s="0">
-        <v>12.335585379975555</v>
+        <v>11.84271928232701</v>
       </c>
       <c r="H9" s="0">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="I9" s="0">
-        <v>5.7008771254956896</v>
+        <v>5.1153364177409353</v>
       </c>
       <c r="J9" s="0">
-        <v>19.5</v>
+        <v>24.25</v>
       </c>
       <c r="K9" s="0">
-        <v>6.0621778264910704</v>
+        <v>5.1861192941672032</v>
       </c>
       <c r="L9" s="0">
-        <v>34.75</v>
+        <v>32</v>
       </c>
       <c r="M9" s="0">
-        <v>10.711170181948686</v>
+        <v>7.2915476180757857</v>
       </c>
       <c r="N9" s="0">
-        <v>96.354627496159779</v>
+        <v>117.15584108946607</v>
       </c>
       <c r="O9" s="0">
-        <v>51.332148006698183</v>
+        <v>43.28518335230283</v>
       </c>
       <c r="P9" s="0">
-        <v>95.194464844370614</v>
+        <v>118.33904970334234</v>
       </c>
       <c r="Q9" s="0">
-        <v>31.337412702988139</v>
+        <v>25.131773917755638</v>
       </c>
     </row>
     <row r="10">
@@ -636,46 +636,46 @@
         <v>6</v>
       </c>
       <c r="D10" s="0">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E10" s="0">
         <v>4</v>
       </c>
       <c r="F10" s="0">
-        <v>22.5</v>
+        <v>41</v>
       </c>
       <c r="G10" s="0">
-        <v>10.267261887507626</v>
+        <v>12.335585379975555</v>
       </c>
       <c r="H10" s="0">
-        <v>2.75</v>
+        <v>11</v>
       </c>
       <c r="I10" s="0">
-        <v>1.4930394055974097</v>
+        <v>5.7008771254956896</v>
       </c>
       <c r="J10" s="0">
-        <v>12.25</v>
+        <v>19.5</v>
       </c>
       <c r="K10" s="0">
-        <v>6.2898728127045622</v>
+        <v>6.0621778264910704</v>
       </c>
       <c r="L10" s="0">
-        <v>36.25</v>
+        <v>34.75</v>
       </c>
       <c r="M10" s="0">
-        <v>18.372874026673127</v>
+        <v>10.711170181948686</v>
       </c>
       <c r="N10" s="0">
-        <v>127.1013737060041</v>
+        <v>96.354627496159779</v>
       </c>
       <c r="O10" s="0">
-        <v>40.645243770063978</v>
+        <v>51.332148006698183</v>
       </c>
       <c r="P10" s="0">
-        <v>61.021358264764288</v>
+        <v>95.194464844370614</v>
       </c>
       <c r="Q10" s="0">
-        <v>32.518021178612607</v>
+        <v>31.337412702988139</v>
       </c>
     </row>
     <row r="11">
@@ -689,7 +689,7 @@
         <v>6</v>
       </c>
       <c r="D11" s="0">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E11" s="0">
         <v>4</v>
@@ -698,37 +698,37 @@
         <v>22.5</v>
       </c>
       <c r="G11" s="0">
-        <v>7.5</v>
+        <v>10.267261887507626</v>
       </c>
       <c r="H11" s="0">
-        <v>3.5</v>
+        <v>2.75</v>
       </c>
       <c r="I11" s="0">
-        <v>0.6454972243679028</v>
+        <v>1.4930394055974097</v>
       </c>
       <c r="J11" s="0">
         <v>12.25</v>
       </c>
       <c r="K11" s="0">
-        <v>4.3851073723076235</v>
+        <v>6.2898728127045622</v>
       </c>
       <c r="L11" s="0">
-        <v>24.25</v>
+        <v>36.25</v>
       </c>
       <c r="M11" s="0">
-        <v>5.4217924465377072</v>
+        <v>18.372874026673127</v>
       </c>
       <c r="N11" s="0">
-        <v>222.01591666666653</v>
+        <v>127.1013737060041</v>
       </c>
       <c r="O11" s="0">
-        <v>193.05319351500069</v>
+        <v>40.645243770063978</v>
       </c>
       <c r="P11" s="0">
-        <v>60.442991085239044</v>
+        <v>61.021358264764288</v>
       </c>
       <c r="Q11" s="0">
-        <v>22.810139304691134</v>
+        <v>32.518021178612607</v>
       </c>
     </row>
     <row r="12">
@@ -742,46 +742,46 @@
         <v>6</v>
       </c>
       <c r="D12" s="0">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E12" s="0">
         <v>4</v>
       </c>
       <c r="F12" s="0">
-        <v>26.5</v>
+        <v>22.5</v>
       </c>
       <c r="G12" s="0">
-        <v>5.634713834792322</v>
+        <v>7.5</v>
       </c>
       <c r="H12" s="0">
-        <v>6.75</v>
+        <v>3.5</v>
       </c>
       <c r="I12" s="0">
-        <v>2.809952550014561</v>
+        <v>0.6454972243679028</v>
       </c>
       <c r="J12" s="0">
-        <v>15.5</v>
+        <v>12.25</v>
       </c>
       <c r="K12" s="0">
-        <v>3.4034296427770228</v>
+        <v>4.3851073723076235</v>
       </c>
       <c r="L12" s="0">
-        <v>32.5</v>
+        <v>24.25</v>
       </c>
       <c r="M12" s="0">
-        <v>10.242883708539635</v>
+        <v>5.4217924465377072</v>
       </c>
       <c r="N12" s="0">
-        <v>131.38006477732793</v>
+        <v>222.01591666666653</v>
       </c>
       <c r="O12" s="0">
-        <v>34.427451776658629</v>
+        <v>193.05319351500069</v>
       </c>
       <c r="P12" s="0">
-        <v>74.505491586046276</v>
+        <v>60.442991085239044</v>
       </c>
       <c r="Q12" s="0">
-        <v>16.548829800403684</v>
+        <v>22.810139304691134</v>
       </c>
     </row>
     <row r="13">
@@ -792,45 +792,49 @@
         <v>4</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="D13" s="0">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E13" s="0">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F13" s="0">
-        <v>22.333333333333332</v>
+        <v>26.5</v>
       </c>
       <c r="G13" s="0">
-        <v>5.8404718226450774</v>
+        <v>5.634713834792322</v>
       </c>
       <c r="H13" s="0">
-        <v>11.333333333333334</v>
+        <v>6.75</v>
       </c>
       <c r="I13" s="0">
-        <v>2.9059326290271157</v>
+        <v>2.809952550014561</v>
       </c>
       <c r="J13" s="0">
-        <v>11</v>
+        <v>15.5</v>
       </c>
       <c r="K13" s="0">
-        <v>0.57735026918962584</v>
+        <v>3.4034296427770228</v>
       </c>
       <c r="L13" s="0">
-        <v>42.666666666666664</v>
+        <v>32.5</v>
       </c>
       <c r="M13" s="0">
-        <v>13.245544324203685</v>
-      </c>
-      <c r="N13" s="0"/>
-      <c r="O13" s="0"/>
+        <v>10.242883708539635</v>
+      </c>
+      <c r="N13" s="0">
+        <v>131.38006477732793</v>
+      </c>
+      <c r="O13" s="0">
+        <v>34.427451776658629</v>
+      </c>
       <c r="P13" s="0">
-        <v>0</v>
+        <v>74.505491586046276</v>
       </c>
       <c r="Q13" s="0">
-        <v>0</v>
+        <v>16.548829800403684</v>
       </c>
     </row>
     <row r="14">
@@ -841,49 +845,49 @@
         <v>4</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="D14" s="0">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="E14" s="0">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F14" s="0">
-        <v>17.666666666666668</v>
+        <v>18.75</v>
       </c>
       <c r="G14" s="0">
-        <v>17.169093679567879</v>
+        <v>3.0652623596249202</v>
       </c>
       <c r="H14" s="0">
-        <v>0.33333333333333331</v>
+        <v>5</v>
       </c>
       <c r="I14" s="0">
-        <v>0.33333333333333337</v>
+        <v>1.1547005383792515</v>
       </c>
       <c r="J14" s="0">
-        <v>11</v>
+        <v>12.75</v>
       </c>
       <c r="K14" s="0">
-        <v>10.503967504392488</v>
+        <v>3.5910769044025406</v>
       </c>
       <c r="L14" s="0">
-        <v>66</v>
+        <v>28.75</v>
       </c>
       <c r="M14" s="0">
-        <v>23.797758998135379</v>
+        <v>8.429857650043683</v>
       </c>
       <c r="N14" s="0">
-        <v>147.12807692307683</v>
+        <v>84.06647228506796</v>
       </c>
       <c r="O14" s="0">
-        <v>124.50807692307683</v>
+        <v>62.929509334137244</v>
       </c>
       <c r="P14" s="0">
-        <v>59.720951008334417</v>
+        <v>61.849217835022522</v>
       </c>
       <c r="Q14" s="0">
-        <v>57.017462445790393</v>
+        <v>17.736049292746888</v>
       </c>
     </row>
     <row r="15">
@@ -894,49 +898,49 @@
         <v>4</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="D15" s="0">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="E15" s="0">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F15" s="0">
-        <v>15.666666666666666</v>
+        <v>32.5</v>
       </c>
       <c r="G15" s="0">
-        <v>7.4236858171066959</v>
+        <v>2.9011491975882016</v>
       </c>
       <c r="H15" s="0">
-        <v>6.666666666666667</v>
+        <v>10.75</v>
       </c>
       <c r="I15" s="0">
-        <v>6.666666666666667</v>
+        <v>3.0379543555930306</v>
       </c>
       <c r="J15" s="0">
-        <v>9.6666666666666661</v>
+        <v>19.25</v>
       </c>
       <c r="K15" s="0">
-        <v>4.4845413490245702</v>
+        <v>4.1907636535600528</v>
       </c>
       <c r="L15" s="0">
-        <v>62</v>
+        <v>31.75</v>
       </c>
       <c r="M15" s="0">
-        <v>15.176736583776281</v>
+        <v>9.4019058351662572</v>
       </c>
       <c r="N15" s="0">
-        <v>50.378703703703508</v>
+        <v>24.006184269162141</v>
       </c>
       <c r="O15" s="0">
-        <v>27.410077455651834</v>
+        <v>6.6001030137059988</v>
       </c>
       <c r="P15" s="0">
-        <v>56.2978047256697</v>
+        <v>93.614660815289724</v>
       </c>
       <c r="Q15" s="0">
-        <v>26.47196134009884</v>
+        <v>21.101475075908073</v>
       </c>
     </row>
     <row r="16">
@@ -947,49 +951,49 @@
         <v>4</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="D16" s="0">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="E16" s="0">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F16" s="0">
-        <v>36.666666666666664</v>
+        <v>26.25</v>
       </c>
       <c r="G16" s="0">
-        <v>9.0615181460454579</v>
+        <v>6.101570835995159</v>
       </c>
       <c r="H16" s="0">
-        <v>8.3333333333333339</v>
+        <v>4.5</v>
       </c>
       <c r="I16" s="0">
-        <v>6.8879927732572757</v>
+        <v>2.0207259421636903</v>
       </c>
       <c r="J16" s="0">
-        <v>23.333333333333332</v>
+        <v>13.75</v>
       </c>
       <c r="K16" s="0">
-        <v>6.1734197258173786</v>
+        <v>4.0901303972693421</v>
       </c>
       <c r="L16" s="0">
-        <v>37.333333333333336</v>
+        <v>31.25</v>
       </c>
       <c r="M16" s="0">
-        <v>18.351506144667738</v>
+        <v>13.021616643105418</v>
       </c>
       <c r="N16" s="0">
-        <v>171.12352130325806</v>
+        <v>113.79227380952379</v>
       </c>
       <c r="O16" s="0">
-        <v>92.757489371524173</v>
+        <v>91.069599551942488</v>
       </c>
       <c r="P16" s="0">
-        <v>131.14162865217881</v>
+        <v>66.662089047143738</v>
       </c>
       <c r="Q16" s="0">
-        <v>31.421736740495735</v>
+        <v>20.270327151133181</v>
       </c>
     </row>
     <row r="17">
@@ -1000,49 +1004,49 @@
         <v>4</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="D17" s="0">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="E17" s="0">
         <v>4</v>
       </c>
       <c r="F17" s="0">
-        <v>49.75</v>
+        <v>28.75</v>
       </c>
       <c r="G17" s="0">
-        <v>32.208629795962032</v>
+        <v>4.4791182167922292</v>
       </c>
       <c r="H17" s="0">
-        <v>3.25</v>
+        <v>6.25</v>
       </c>
       <c r="I17" s="0">
-        <v>2.6259918760981216</v>
+        <v>3.4247870980057527</v>
       </c>
       <c r="J17" s="0">
-        <v>27.25</v>
+        <v>14.75</v>
       </c>
       <c r="K17" s="0">
-        <v>14.642261892663077</v>
+        <v>3.1983068437325812</v>
       </c>
       <c r="L17" s="0">
-        <v>33</v>
+        <v>30.25</v>
       </c>
       <c r="M17" s="0">
-        <v>9.8064604555704342</v>
+        <v>10.061270628835439</v>
       </c>
       <c r="N17" s="0">
-        <v>194.54360256410257</v>
+        <v>115.96953869047618</v>
       </c>
       <c r="O17" s="0">
-        <v>47.180177760276493</v>
+        <v>70.291276155621318</v>
       </c>
       <c r="P17" s="0">
-        <v>151.34939789819879</v>
+        <v>71.380602106367732</v>
       </c>
       <c r="Q17" s="0">
-        <v>78.840681649188383</v>
+        <v>15.948296070680044</v>
       </c>
     </row>
     <row r="18">
@@ -1056,46 +1060,42 @@
         <v>22</v>
       </c>
       <c r="D18" s="0">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E18" s="0">
         <v>3</v>
       </c>
       <c r="F18" s="0">
-        <v>39.333333333333336</v>
+        <v>22.333333333333332</v>
       </c>
       <c r="G18" s="0">
-        <v>13.017082793177757</v>
+        <v>5.8404718226450774</v>
       </c>
       <c r="H18" s="0">
         <v>11.333333333333334</v>
       </c>
       <c r="I18" s="0">
-        <v>10.333333333333334</v>
+        <v>2.9059326290271157</v>
       </c>
       <c r="J18" s="0">
-        <v>24.666666666666668</v>
+        <v>11</v>
       </c>
       <c r="K18" s="0">
-        <v>8.6666666666666679</v>
+        <v>0.57735026918962584</v>
       </c>
       <c r="L18" s="0">
-        <v>38.666666666666664</v>
+        <v>42.666666666666664</v>
       </c>
       <c r="M18" s="0">
-        <v>1.2018504251546631</v>
-      </c>
-      <c r="N18" s="0">
-        <v>193.94226190476198</v>
-      </c>
-      <c r="O18" s="0">
-        <v>64.546990462261391</v>
-      </c>
+        <v>13.245544324203685</v>
+      </c>
+      <c r="N18" s="0"/>
+      <c r="O18" s="0"/>
       <c r="P18" s="0">
-        <v>135.36147039755053</v>
+        <v>0</v>
       </c>
       <c r="Q18" s="0">
-        <v>47.607984224371108</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -1109,46 +1109,46 @@
         <v>22</v>
       </c>
       <c r="D19" s="0">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E19" s="0">
         <v>3</v>
       </c>
       <c r="F19" s="0">
-        <v>20.666666666666668</v>
+        <v>17.666666666666668</v>
       </c>
       <c r="G19" s="0">
-        <v>7.2188026092359054</v>
+        <v>17.169093679567879</v>
       </c>
       <c r="H19" s="0">
-        <v>2.3333333333333335</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="I19" s="0">
-        <v>1.8559214542766742</v>
+        <v>0.33333333333333337</v>
       </c>
       <c r="J19" s="0">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="K19" s="0">
-        <v>3.2145502536643185</v>
+        <v>10.503967504392488</v>
       </c>
       <c r="L19" s="0">
-        <v>28.333333333333332</v>
+        <v>66</v>
       </c>
       <c r="M19" s="0">
-        <v>15.719768163402129</v>
+        <v>23.797758998135379</v>
       </c>
       <c r="N19" s="0">
-        <v>141.20233333333331</v>
+        <v>147.12807692307683</v>
       </c>
       <c r="O19" s="0">
-        <v>26.809651749433957</v>
+        <v>124.50807692307683</v>
       </c>
       <c r="P19" s="0">
-        <v>89.13695704326004</v>
+        <v>59.720951008334417</v>
       </c>
       <c r="Q19" s="0">
-        <v>19.774548598661202</v>
+        <v>57.017462445790393</v>
       </c>
     </row>
     <row r="20">
@@ -1162,46 +1162,46 @@
         <v>22</v>
       </c>
       <c r="D20" s="0">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E20" s="0">
         <v>3</v>
       </c>
       <c r="F20" s="0">
-        <v>26.666666666666668</v>
+        <v>15.666666666666666</v>
       </c>
       <c r="G20" s="0">
-        <v>9.9554563487120529</v>
+        <v>7.4236858171066959</v>
       </c>
       <c r="H20" s="0">
-        <v>4.666666666666667</v>
+        <v>6.666666666666667</v>
       </c>
       <c r="I20" s="0">
-        <v>4.1766546953805559</v>
+        <v>6.666666666666667</v>
       </c>
       <c r="J20" s="0">
-        <v>19.333333333333332</v>
+        <v>9.6666666666666661</v>
       </c>
       <c r="K20" s="0">
-        <v>5.7831171909658243</v>
+        <v>4.4845413490245702</v>
       </c>
       <c r="L20" s="0">
-        <v>34.666666666666664</v>
+        <v>62</v>
       </c>
       <c r="M20" s="0">
-        <v>11.89304184994085</v>
+        <v>15.176736583776281</v>
       </c>
       <c r="N20" s="0">
-        <v>103.55441798941801</v>
+        <v>50.378703703703508</v>
       </c>
       <c r="O20" s="0">
-        <v>31.842857207617705</v>
+        <v>27.410077455651834</v>
       </c>
       <c r="P20" s="0">
-        <v>108.15475427996523</v>
+        <v>56.2978047256697</v>
       </c>
       <c r="Q20" s="0">
-        <v>33.800915352693998</v>
+        <v>26.47196134009884</v>
       </c>
     </row>
     <row r="21">
@@ -1215,46 +1215,46 @@
         <v>22</v>
       </c>
       <c r="D21" s="0">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E21" s="0">
         <v>3</v>
       </c>
       <c r="F21" s="0">
-        <v>14.666666666666666</v>
+        <v>36.666666666666664</v>
       </c>
       <c r="G21" s="0">
-        <v>2.728450923957483</v>
+        <v>9.0615181460454579</v>
       </c>
       <c r="H21" s="0">
-        <v>6.333333333333333</v>
+        <v>8.3333333333333339</v>
       </c>
       <c r="I21" s="0">
-        <v>3.2829526005987018</v>
+        <v>6.8879927732572757</v>
       </c>
       <c r="J21" s="0">
-        <v>12.333333333333334</v>
+        <v>23.333333333333332</v>
       </c>
       <c r="K21" s="0">
-        <v>2.8480012484391777</v>
+        <v>6.1734197258173786</v>
       </c>
       <c r="L21" s="0">
-        <v>24.333333333333332</v>
+        <v>37.333333333333336</v>
       </c>
       <c r="M21" s="0">
-        <v>9.4044906531105923</v>
+        <v>18.351506144667738</v>
       </c>
       <c r="N21" s="0">
-        <v>259.80317460317463</v>
+        <v>171.12352130325806</v>
       </c>
       <c r="O21" s="0">
-        <v>181.81741983243114</v>
+        <v>92.757489371524173</v>
       </c>
       <c r="P21" s="0">
-        <v>67.453179995532537</v>
+        <v>131.14162865217881</v>
       </c>
       <c r="Q21" s="0">
-        <v>14.024567676957011</v>
+        <v>31.421736740495735</v>
       </c>
     </row>
     <row r="22">
@@ -1268,46 +1268,46 @@
         <v>22</v>
       </c>
       <c r="D22" s="0">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E22" s="0">
         <v>3</v>
       </c>
       <c r="F22" s="0">
-        <v>10.333333333333334</v>
+        <v>62.333333333333336</v>
       </c>
       <c r="G22" s="0">
-        <v>2.3333333333333335</v>
+        <v>41.929835572192637</v>
       </c>
       <c r="H22" s="0">
-        <v>1.3333333333333333</v>
+        <v>4.333333333333333</v>
       </c>
       <c r="I22" s="0">
-        <v>0.88191710368819698</v>
+        <v>3.3829638550307402</v>
       </c>
       <c r="J22" s="0">
-        <v>9</v>
+        <v>33.333333333333336</v>
       </c>
       <c r="K22" s="0">
-        <v>1</v>
+        <v>18.835545592782221</v>
       </c>
       <c r="L22" s="0">
-        <v>35.333333333333336</v>
+        <v>25.666666666666668</v>
       </c>
       <c r="M22" s="0">
-        <v>14.847371634213394</v>
+        <v>9.207484877955423</v>
       </c>
       <c r="N22" s="0">
-        <v>187.92211640211642</v>
+        <v>154.30480341880343</v>
       </c>
       <c r="O22" s="0">
-        <v>107.7609416840225</v>
+        <v>34.836998057684639</v>
       </c>
       <c r="P22" s="0">
-        <v>49.909091132794707</v>
+        <v>184.54345251674729</v>
       </c>
       <c r="Q22" s="0">
-        <v>6.5701566750317086</v>
+        <v>101.13365237041019</v>
       </c>
     </row>
     <row r="23">
@@ -1321,572 +1321,576 @@
         <v>22</v>
       </c>
       <c r="D23" s="0">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E23" s="0">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F23" s="0">
-        <v>54.333333333333336</v>
+        <v>12</v>
       </c>
       <c r="G23" s="0">
-        <v>5.0442486501405197</v>
+        <v>0</v>
       </c>
       <c r="H23" s="0">
-        <v>7.666666666666667</v>
+        <v>0</v>
       </c>
       <c r="I23" s="0">
-        <v>3.2829526005987018</v>
+        <v>0</v>
       </c>
       <c r="J23" s="0">
-        <v>38.333333333333336</v>
+        <v>9</v>
       </c>
       <c r="K23" s="0">
-        <v>3.8441875315569325</v>
+        <v>0</v>
       </c>
       <c r="L23" s="0">
-        <v>40.333333333333336</v>
+        <v>55</v>
       </c>
       <c r="M23" s="0">
-        <v>16.333333333333332</v>
+        <v>0</v>
       </c>
       <c r="N23" s="0">
-        <v>242.66604797979792</v>
+        <v>315.25999999999999</v>
       </c>
       <c r="O23" s="0">
-        <v>85.094911956049671</v>
+        <v>0</v>
       </c>
       <c r="P23" s="0">
-        <v>208.23127448771447</v>
+        <v>51.767234042553206</v>
       </c>
       <c r="Q23" s="0">
-        <v>23.504791614783297</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B24" s="0" t="s">
         <v>4</v>
       </c>
       <c r="C24" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" s="0">
         <v>6</v>
       </c>
-      <c r="D24" s="0">
-        <v>0</v>
-      </c>
       <c r="E24" s="0">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F24" s="0">
-        <v>19.25</v>
+        <v>39.333333333333336</v>
       </c>
       <c r="G24" s="0">
-        <v>6.2898728127045622</v>
+        <v>13.017082793177757</v>
       </c>
       <c r="H24" s="0">
-        <v>8</v>
+        <v>11.333333333333334</v>
       </c>
       <c r="I24" s="0">
-        <v>2.6770630673681683</v>
+        <v>10.333333333333334</v>
       </c>
       <c r="J24" s="0">
-        <v>8.75</v>
+        <v>24.666666666666668</v>
       </c>
       <c r="K24" s="0">
-        <v>3.0923292192132452</v>
+        <v>8.6666666666666679</v>
       </c>
       <c r="L24" s="0">
-        <v>69</v>
+        <v>38.666666666666664</v>
       </c>
       <c r="M24" s="0">
-        <v>15.016657417681207</v>
-      </c>
-      <c r="N24" s="0"/>
-      <c r="O24" s="0"/>
+        <v>1.2018504251546631</v>
+      </c>
+      <c r="N24" s="0">
+        <v>193.94226190476198</v>
+      </c>
+      <c r="O24" s="0">
+        <v>64.546990462261391</v>
+      </c>
       <c r="P24" s="0">
-        <v>0</v>
+        <v>135.36147039755053</v>
       </c>
       <c r="Q24" s="0">
-        <v>0</v>
+        <v>47.607984224371108</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B25" s="0" t="s">
         <v>4</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="D25" s="0">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E25" s="0">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F25" s="0">
-        <v>26.5</v>
+        <v>20.666666666666668</v>
       </c>
       <c r="G25" s="0">
-        <v>14.642973286415115</v>
+        <v>7.2188026092359054</v>
       </c>
       <c r="H25" s="0">
-        <v>4.75</v>
+        <v>2.3333333333333335</v>
       </c>
       <c r="I25" s="0">
-        <v>1.8874586088176875</v>
+        <v>1.8559214542766742</v>
       </c>
       <c r="J25" s="0">
-        <v>14.25</v>
+        <v>16</v>
       </c>
       <c r="K25" s="0">
-        <v>5.1700257897487001</v>
+        <v>3.2145502536643185</v>
       </c>
       <c r="L25" s="0">
-        <v>94</v>
+        <v>28.333333333333332</v>
       </c>
       <c r="M25" s="0">
-        <v>19.131126469708992</v>
+        <v>15.719768163402129</v>
       </c>
       <c r="N25" s="0">
-        <v>22.168641025641094</v>
+        <v>141.20233333333331</v>
       </c>
       <c r="O25" s="0">
-        <v>10.533023318956069</v>
+        <v>26.809651749433957</v>
       </c>
       <c r="P25" s="0">
-        <v>49.994060601563049</v>
+        <v>89.13695704326004</v>
       </c>
       <c r="Q25" s="0">
-        <v>19.870402113019829</v>
+        <v>19.774548598661202</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B26" s="0" t="s">
         <v>4</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="D26" s="0">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E26" s="0">
         <v>3</v>
       </c>
       <c r="F26" s="0">
-        <v>31</v>
+        <v>26.666666666666668</v>
       </c>
       <c r="G26" s="0">
-        <v>10.583005244258363</v>
+        <v>9.9554563487120529</v>
       </c>
       <c r="H26" s="0">
-        <v>8.3333333333333339</v>
+        <v>4.666666666666667</v>
       </c>
       <c r="I26" s="0">
-        <v>3.3333333333333335</v>
+        <v>4.1766546953805559</v>
       </c>
       <c r="J26" s="0">
-        <v>15.333333333333334</v>
+        <v>19.333333333333332</v>
       </c>
       <c r="K26" s="0">
-        <v>4.0960685758148365</v>
+        <v>5.7831171909658243</v>
       </c>
       <c r="L26" s="0">
-        <v>50.666666666666664</v>
+        <v>34.666666666666664</v>
       </c>
       <c r="M26" s="0">
-        <v>6.6916199666282443</v>
+        <v>11.89304184994085</v>
       </c>
       <c r="N26" s="0">
-        <v>33.977886002886017</v>
+        <v>103.55441798941801</v>
       </c>
       <c r="O26" s="0">
-        <v>13.172894507551444</v>
+        <v>31.842857207617705</v>
       </c>
       <c r="P26" s="0">
-        <v>53.720718787482781</v>
+        <v>108.15475427996523</v>
       </c>
       <c r="Q26" s="0">
-        <v>16.626710579297754</v>
+        <v>33.800915352693998</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B27" s="0" t="s">
         <v>4</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="D27" s="0">
+        <v>9</v>
+      </c>
+      <c r="E27" s="0">
         <v>3</v>
       </c>
-      <c r="E27" s="0">
-        <v>4</v>
-      </c>
       <c r="F27" s="0">
-        <v>52</v>
+        <v>14.666666666666666</v>
       </c>
       <c r="G27" s="0">
-        <v>13.90443574307614</v>
+        <v>2.728450923957483</v>
       </c>
       <c r="H27" s="0">
-        <v>28</v>
+        <v>6.333333333333333</v>
       </c>
       <c r="I27" s="0">
-        <v>16.140012391568973</v>
+        <v>3.2829526005987018</v>
       </c>
       <c r="J27" s="0">
-        <v>32.75</v>
+        <v>12.333333333333334</v>
       </c>
       <c r="K27" s="0">
-        <v>7.7714756213561742</v>
+        <v>2.8480012484391777</v>
       </c>
       <c r="L27" s="0">
-        <v>85.25</v>
+        <v>24.333333333333332</v>
       </c>
       <c r="M27" s="0">
-        <v>17.899604278679831</v>
+        <v>9.4044906531105923</v>
       </c>
       <c r="N27" s="0">
-        <v>65.366862207602395</v>
+        <v>259.80317460317463</v>
       </c>
       <c r="O27" s="0">
-        <v>32.454443000967174</v>
+        <v>181.81741983243114</v>
       </c>
       <c r="P27" s="0">
-        <v>112.19959175674629</v>
+        <v>67.453179995532537</v>
       </c>
       <c r="Q27" s="0">
-        <v>27.388405886137765</v>
+        <v>14.024567676957011</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B28" s="0" t="s">
         <v>4</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="D28" s="0">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E28" s="0">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F28" s="0">
-        <v>34.5</v>
+        <v>10.333333333333334</v>
       </c>
       <c r="G28" s="0">
-        <v>7.9529868602934339</v>
+        <v>2.3333333333333335</v>
       </c>
       <c r="H28" s="0">
-        <v>10.666666666666666</v>
+        <v>1.3333333333333333</v>
       </c>
       <c r="I28" s="0">
-        <v>3.2214558475598856</v>
+        <v>0.88191710368819698</v>
       </c>
       <c r="J28" s="0">
-        <v>23.833333333333332</v>
+        <v>9</v>
       </c>
       <c r="K28" s="0">
-        <v>6.4777396606463817</v>
+        <v>1</v>
       </c>
       <c r="L28" s="0">
-        <v>49.666666666666664</v>
+        <v>35.333333333333336</v>
       </c>
       <c r="M28" s="0">
-        <v>6.6916199666282434</v>
+        <v>14.847371634213394</v>
       </c>
       <c r="N28" s="0">
-        <v>87.773193392255891</v>
+        <v>187.92211640211642</v>
       </c>
       <c r="O28" s="0">
-        <v>37.660379526578986</v>
+        <v>107.7609416840225</v>
       </c>
       <c r="P28" s="0">
-        <v>78.719213084333219</v>
+        <v>49.909091132794707</v>
       </c>
       <c r="Q28" s="0">
-        <v>20.497351046408252</v>
+        <v>6.5701566750317086</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B29" s="0" t="s">
         <v>4</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="D29" s="0">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="E29" s="0">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F29" s="0">
-        <v>24.5</v>
+        <v>54.333333333333336</v>
       </c>
       <c r="G29" s="0">
-        <v>4.7346242371139304</v>
+        <v>5.0442486501405197</v>
       </c>
       <c r="H29" s="0">
-        <v>9.25</v>
+        <v>7.666666666666667</v>
       </c>
       <c r="I29" s="0">
-        <v>1.7017148213885114</v>
+        <v>3.2829526005987018</v>
       </c>
       <c r="J29" s="0">
-        <v>20.25</v>
+        <v>38.333333333333336</v>
       </c>
       <c r="K29" s="0">
-        <v>3.2242570203588508</v>
+        <v>3.8441875315569325</v>
       </c>
       <c r="L29" s="0">
-        <v>43.75</v>
+        <v>40.333333333333336</v>
       </c>
       <c r="M29" s="0">
-        <v>11.685995892520243</v>
+        <v>16.333333333333332</v>
       </c>
       <c r="N29" s="0">
-        <v>58.356144480519482</v>
+        <v>242.66604797979792</v>
       </c>
       <c r="O29" s="0">
-        <v>39.025444277436456</v>
+        <v>85.094911956049671</v>
       </c>
       <c r="P29" s="0">
-        <v>66.345643537008328</v>
+        <v>208.23127448771447</v>
       </c>
       <c r="Q29" s="0">
-        <v>10.408746001378843</v>
+        <v>23.504791614783297</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B30" s="0" t="s">
         <v>4</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="D30" s="0">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E30" s="0">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F30" s="0">
-        <v>24.75</v>
+        <v>29.333333333333332</v>
       </c>
       <c r="G30" s="0">
-        <v>5.5883062430996624</v>
+        <v>8.192137151629673</v>
       </c>
       <c r="H30" s="0">
-        <v>12.5</v>
+        <v>5.666666666666667</v>
       </c>
       <c r="I30" s="0">
-        <v>1.8929694486000912</v>
+        <v>3.4801021696368499</v>
       </c>
       <c r="J30" s="0">
-        <v>19.5</v>
+        <v>20</v>
       </c>
       <c r="K30" s="0">
-        <v>4.2914643965279113</v>
+        <v>4.1633319989322652</v>
       </c>
       <c r="L30" s="0">
-        <v>42.5</v>
+        <v>20.666666666666668</v>
       </c>
       <c r="M30" s="0">
-        <v>5.634713834792322</v>
+        <v>5.9254629448770597</v>
       </c>
       <c r="N30" s="0">
-        <v>98.323651789386957</v>
+        <v>475.97514814814809</v>
       </c>
       <c r="O30" s="0">
-        <v>43.959531955662413</v>
+        <v>189.44740330327915</v>
       </c>
       <c r="P30" s="0">
-        <v>64.777571457735448</v>
+        <v>107.74190013548792</v>
       </c>
       <c r="Q30" s="0">
-        <v>15.103410376999443</v>
+        <v>21.020762780909553</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B31" s="0" t="s">
         <v>4</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="D31" s="0">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E31" s="0">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F31" s="0">
-        <v>22.75</v>
+        <v>37.666666666666664</v>
       </c>
       <c r="G31" s="0">
-        <v>3.6827299656640586</v>
+        <v>8.6666666666666679</v>
       </c>
       <c r="H31" s="0">
-        <v>8.75</v>
+        <v>12.666666666666666</v>
       </c>
       <c r="I31" s="0">
-        <v>2.6887109674836132</v>
+        <v>5.3644923131436943</v>
       </c>
       <c r="J31" s="0">
-        <v>15.25</v>
+        <v>26.333333333333332</v>
       </c>
       <c r="K31" s="0">
-        <v>2.2126530078919591</v>
+        <v>6.8394281762277309</v>
       </c>
       <c r="L31" s="0">
-        <v>47</v>
+        <v>33.333333333333336</v>
       </c>
       <c r="M31" s="0">
-        <v>12.935738607954837</v>
+        <v>4.1766546953805559</v>
       </c>
       <c r="N31" s="0">
-        <v>157.92080176767675</v>
+        <v>304.37674857549854</v>
       </c>
       <c r="O31" s="0">
-        <v>83.227737171056702</v>
+        <v>157.7987128212724</v>
       </c>
       <c r="P31" s="0">
-        <v>50.256551304898892</v>
+        <v>143.33137566805161</v>
       </c>
       <c r="Q31" s="0">
-        <v>7.7511695070748141</v>
+        <v>38.686492556508803</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B32" s="0" t="s">
         <v>4</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="D32" s="0">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E32" s="0">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F32" s="0">
-        <v>29.5</v>
+        <v>17</v>
       </c>
       <c r="G32" s="0">
-        <v>4.1733280085163047</v>
+        <v>5.2915026221291814</v>
       </c>
       <c r="H32" s="0">
-        <v>5.75</v>
+        <v>4.333333333333333</v>
       </c>
       <c r="I32" s="0">
-        <v>1.4930394055974097</v>
+        <v>4.3333333333333339</v>
       </c>
       <c r="J32" s="0">
-        <v>19.75</v>
+        <v>13.666666666666666</v>
       </c>
       <c r="K32" s="0">
-        <v>2.2867371223353739</v>
+        <v>3.7564758898615485</v>
       </c>
       <c r="L32" s="0">
-        <v>50.75</v>
+        <v>19.666666666666668</v>
       </c>
       <c r="M32" s="0">
-        <v>16.131620088096131</v>
+        <v>9.5277372853043012</v>
       </c>
       <c r="N32" s="0">
-        <v>65.46980357142867</v>
+        <v>375.290202020202</v>
       </c>
       <c r="O32" s="0">
-        <v>42.191087062516566</v>
+        <v>169.71056913701193</v>
       </c>
       <c r="P32" s="0">
-        <v>64.147899335807864</v>
+        <v>74.186329358820686</v>
       </c>
       <c r="Q32" s="0">
-        <v>5.9704849097917378</v>
+        <v>21.122182496662028</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B33" s="0" t="s">
         <v>4</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="D33" s="0">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E33" s="0">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F33" s="0">
-        <v>26.25</v>
+        <v>26.666666666666668</v>
       </c>
       <c r="G33" s="0">
-        <v>6.3688696014284982</v>
+        <v>12.719189352225943</v>
       </c>
       <c r="H33" s="0">
-        <v>5</v>
+        <v>4.666666666666667</v>
       </c>
       <c r="I33" s="0">
-        <v>1.2909944487358056</v>
+        <v>1.4529663145135578</v>
       </c>
       <c r="J33" s="0">
-        <v>19.5</v>
+        <v>19.666666666666668</v>
       </c>
       <c r="K33" s="0">
-        <v>4.4253060157839181</v>
+        <v>8.6666666666666679</v>
       </c>
       <c r="L33" s="0">
-        <v>52.25</v>
+        <v>29.333333333333332</v>
       </c>
       <c r="M33" s="0">
-        <v>7.3979163733220625</v>
+        <v>15.835964693626272</v>
       </c>
       <c r="N33" s="0">
-        <v>76.725373376623381</v>
+        <v>313.52541666666667</v>
       </c>
       <c r="O33" s="0">
-        <v>69.106430857045268</v>
+        <v>156.1473641513798</v>
       </c>
       <c r="P33" s="0">
-        <v>63.31241883365562</v>
+        <v>104.33947060573014</v>
       </c>
       <c r="Q33" s="0">
-        <v>13.870452293565409</v>
+        <v>43.275275321843061</v>
       </c>
     </row>
     <row r="34">
@@ -1900,46 +1904,42 @@
         <v>6</v>
       </c>
       <c r="D34" s="0">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="E34" s="0">
         <v>4</v>
       </c>
       <c r="F34" s="0">
-        <v>25.75</v>
+        <v>19.25</v>
       </c>
       <c r="G34" s="0">
-        <v>3.966001344763598</v>
+        <v>6.2898728127045622</v>
       </c>
       <c r="H34" s="0">
-        <v>4.5</v>
+        <v>8</v>
       </c>
       <c r="I34" s="0">
-        <v>1.9364916731037085</v>
+        <v>2.6770630673681683</v>
       </c>
       <c r="J34" s="0">
-        <v>20.25</v>
+        <v>8.75</v>
       </c>
       <c r="K34" s="0">
-        <v>2.0155644370746373</v>
+        <v>3.0923292192132452</v>
       </c>
       <c r="L34" s="0">
-        <v>48.25</v>
+        <v>69</v>
       </c>
       <c r="M34" s="0">
-        <v>11.360567767501763</v>
-      </c>
-      <c r="N34" s="0">
-        <v>51.138666666666744</v>
-      </c>
-      <c r="O34" s="0">
-        <v>40.114655891304643</v>
-      </c>
+        <v>15.016657417681207</v>
+      </c>
+      <c r="N34" s="0"/>
+      <c r="O34" s="0"/>
       <c r="P34" s="0">
-        <v>64.238335695371177</v>
+        <v>0</v>
       </c>
       <c r="Q34" s="0">
-        <v>4.4645526493660395</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35">
@@ -1950,45 +1950,49 @@
         <v>4</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="D35" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E35" s="0">
         <v>4</v>
       </c>
       <c r="F35" s="0">
-        <v>11.5</v>
+        <v>26.5</v>
       </c>
       <c r="G35" s="0">
-        <v>3.378855822118882</v>
+        <v>14.642973286415115</v>
       </c>
       <c r="H35" s="0">
-        <v>5.75</v>
+        <v>4.75</v>
       </c>
       <c r="I35" s="0">
-        <v>1.1086778913041726</v>
+        <v>1.8874586088176875</v>
       </c>
       <c r="J35" s="0">
-        <v>6.75</v>
+        <v>14.25</v>
       </c>
       <c r="K35" s="0">
-        <v>1.973786547054502</v>
+        <v>5.1700257897487001</v>
       </c>
       <c r="L35" s="0">
-        <v>26.75</v>
+        <v>94</v>
       </c>
       <c r="M35" s="0">
-        <v>2.5289984842489197</v>
-      </c>
-      <c r="N35" s="0"/>
-      <c r="O35" s="0"/>
+        <v>19.131126469708992</v>
+      </c>
+      <c r="N35" s="0">
+        <v>22.168641025641094</v>
+      </c>
+      <c r="O35" s="0">
+        <v>10.533023318956069</v>
+      </c>
       <c r="P35" s="0">
-        <v>0</v>
+        <v>49.994060601563049</v>
       </c>
       <c r="Q35" s="0">
-        <v>0</v>
+        <v>19.870402113019829</v>
       </c>
     </row>
     <row r="36">
@@ -1999,48 +2003,50 @@
         <v>4</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="D36" s="0">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E36" s="0">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F36" s="0">
-        <v>29.75</v>
+        <v>31</v>
       </c>
       <c r="G36" s="0">
-        <v>12.51915199471061</v>
+        <v>10.583005244258363</v>
       </c>
       <c r="H36" s="0">
-        <v>5.5</v>
+        <v>8.3333333333333339</v>
       </c>
       <c r="I36" s="0">
-        <v>2.5331140255951108</v>
+        <v>3.3333333333333335</v>
       </c>
       <c r="J36" s="0">
-        <v>18</v>
+        <v>15.333333333333334</v>
       </c>
       <c r="K36" s="0">
-        <v>6.324555320336759</v>
+        <v>4.0960685758148365</v>
       </c>
       <c r="L36" s="0">
-        <v>49.75</v>
+        <v>50.666666666666664</v>
       </c>
       <c r="M36" s="0">
-        <v>11.678862672937521</v>
+        <v>6.6916199666282443</v>
       </c>
       <c r="N36" s="0">
-        <v>199.02467307692302</v>
+        <v>33.977886002886017</v>
       </c>
       <c r="O36" s="0">
-        <v>83.158139318497049</v>
+        <v>13.172894507551444</v>
       </c>
       <c r="P36" s="0">
-        <v>65535</v>
-      </c>
-      <c r="Q36" s="0"/>
+        <v>53.720718787482781</v>
+      </c>
+      <c r="Q36" s="0">
+        <v>16.626710579297754</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="0" t="s">
@@ -2050,49 +2056,49 @@
         <v>4</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="D37" s="0">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E37" s="0">
         <v>4</v>
       </c>
       <c r="F37" s="0">
-        <v>28.5</v>
+        <v>52</v>
       </c>
       <c r="G37" s="0">
-        <v>8.4606934309980364</v>
+        <v>13.90443574307614</v>
       </c>
       <c r="H37" s="0">
-        <v>4.5</v>
+        <v>28</v>
       </c>
       <c r="I37" s="0">
-        <v>1.0408329997330663</v>
+        <v>16.140012391568973</v>
       </c>
       <c r="J37" s="0">
-        <v>18.25</v>
+        <v>32.75</v>
       </c>
       <c r="K37" s="0">
-        <v>5.5283360968739954</v>
+        <v>7.7714756213561742</v>
       </c>
       <c r="L37" s="0">
-        <v>16.5</v>
+        <v>85.25</v>
       </c>
       <c r="M37" s="0">
-        <v>4.0926763859362252</v>
+        <v>17.899604278679831</v>
       </c>
       <c r="N37" s="0">
-        <v>123.76519444444445</v>
+        <v>65.366862207602395</v>
       </c>
       <c r="O37" s="0">
-        <v>96.563654110602727</v>
+        <v>32.454443000967174</v>
       </c>
       <c r="P37" s="0">
-        <v>57.096024507691922</v>
+        <v>112.19959175674629</v>
       </c>
       <c r="Q37" s="0">
-        <v>17.581199231611976</v>
+        <v>27.388405886137765</v>
       </c>
     </row>
     <row r="38">
@@ -2103,48 +2109,50 @@
         <v>4</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="D38" s="0">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E38" s="0">
         <v>4</v>
       </c>
       <c r="F38" s="0">
-        <v>54.25</v>
+        <v>42.75</v>
       </c>
       <c r="G38" s="0">
-        <v>23.264332499916403</v>
+        <v>9.0496316683792895</v>
       </c>
       <c r="H38" s="0">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="I38" s="0">
-        <v>5.8166427888717163</v>
+        <v>3.7638632635454048</v>
       </c>
       <c r="J38" s="0">
-        <v>37</v>
+        <v>28.25</v>
       </c>
       <c r="K38" s="0">
-        <v>16.416455159382004</v>
+        <v>9.0127224891631208</v>
       </c>
       <c r="L38" s="0">
-        <v>29.25</v>
+        <v>46.25</v>
       </c>
       <c r="M38" s="0">
-        <v>7.1922991224410753</v>
+        <v>8.6156350123868801</v>
       </c>
       <c r="N38" s="0">
-        <v>396.74887121212117</v>
+        <v>103.38541508838385</v>
       </c>
       <c r="O38" s="0">
-        <v>320.97552634128039</v>
+        <v>53.774902697870658</v>
       </c>
       <c r="P38" s="0">
-        <v>65535</v>
-      </c>
-      <c r="Q38" s="0"/>
+        <v>94.238180650650094</v>
+      </c>
+      <c r="Q38" s="0">
+        <v>27.768089178816695</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="0" t="s">
@@ -2154,49 +2162,49 @@
         <v>4</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="D39" s="0">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E39" s="0">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F39" s="0">
-        <v>41.666666666666664</v>
+        <v>18</v>
       </c>
       <c r="G39" s="0">
-        <v>15.730366951995888</v>
+        <v>6.9999999999999991</v>
       </c>
       <c r="H39" s="0">
-        <v>5.166666666666667</v>
+        <v>4</v>
       </c>
       <c r="I39" s="0">
-        <v>1.7779513804126119</v>
+        <v>2</v>
       </c>
       <c r="J39" s="0">
-        <v>33.333333333333336</v>
+        <v>15</v>
       </c>
       <c r="K39" s="0">
-        <v>11.757739767678329</v>
+        <v>5</v>
       </c>
       <c r="L39" s="0">
-        <v>21.333333333333332</v>
+        <v>56.5</v>
       </c>
       <c r="M39" s="0">
-        <v>5.9142013643245006</v>
+        <v>12.5</v>
       </c>
       <c r="N39" s="0">
-        <v>285.32431818181823</v>
+        <v>56.548749999999984</v>
       </c>
       <c r="O39" s="0">
-        <v>180.48152809142471</v>
+        <v>49.615250000000039</v>
       </c>
       <c r="P39" s="0">
-        <v>103.3947270594149</v>
+        <v>47.681277951699471</v>
       </c>
       <c r="Q39" s="0">
-        <v>35.958230595396941</v>
+        <v>15.188489490161004</v>
       </c>
     </row>
     <row r="40">
@@ -2207,7 +2215,7 @@
         <v>4</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="D40" s="0">
         <v>6</v>
@@ -2216,39 +2224,41 @@
         <v>4</v>
       </c>
       <c r="F40" s="0">
-        <v>26</v>
+        <v>24.5</v>
       </c>
       <c r="G40" s="0">
-        <v>9.9582461641931044</v>
+        <v>4.7346242371139304</v>
       </c>
       <c r="H40" s="0">
-        <v>6.75</v>
+        <v>9.25</v>
       </c>
       <c r="I40" s="0">
-        <v>2.6575364531836625</v>
+        <v>1.7017148213885114</v>
       </c>
       <c r="J40" s="0">
-        <v>20.75</v>
+        <v>20.25</v>
       </c>
       <c r="K40" s="0">
-        <v>8.1687922403906601</v>
+        <v>3.2242570203588508</v>
       </c>
       <c r="L40" s="0">
-        <v>22.5</v>
+        <v>43.75</v>
       </c>
       <c r="M40" s="0">
-        <v>4.1932485418030412</v>
+        <v>11.685995892520243</v>
       </c>
       <c r="N40" s="0">
-        <v>347.29934920634918</v>
+        <v>58.356144480519482</v>
       </c>
       <c r="O40" s="0">
-        <v>158.54349546179873</v>
+        <v>39.025444277436456</v>
       </c>
       <c r="P40" s="0">
-        <v>65535</v>
-      </c>
-      <c r="Q40" s="0"/>
+        <v>66.345643537008328</v>
+      </c>
+      <c r="Q40" s="0">
+        <v>10.408746001378843</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="0" t="s">
@@ -2258,7 +2268,7 @@
         <v>4</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="D41" s="0">
         <v>7</v>
@@ -2267,40 +2277,40 @@
         <v>4</v>
       </c>
       <c r="F41" s="0">
-        <v>22.75</v>
+        <v>24.75</v>
       </c>
       <c r="G41" s="0">
-        <v>7.9621500446382782</v>
+        <v>5.5883062430996624</v>
       </c>
       <c r="H41" s="0">
-        <v>3.75</v>
+        <v>12.5</v>
       </c>
       <c r="I41" s="0">
-        <v>1.6520189667999174</v>
+        <v>1.8929694486000912</v>
       </c>
       <c r="J41" s="0">
-        <v>20.25</v>
+        <v>19.5</v>
       </c>
       <c r="K41" s="0">
-        <v>7.2154348448309058</v>
+        <v>4.2914643965279113</v>
       </c>
       <c r="L41" s="0">
-        <v>22.75</v>
+        <v>42.5</v>
       </c>
       <c r="M41" s="0">
-        <v>7.9201746613737418</v>
+        <v>5.634713834792322</v>
       </c>
       <c r="N41" s="0">
-        <v>708.12724358974367</v>
+        <v>98.323651789386957</v>
       </c>
       <c r="O41" s="0">
-        <v>561.21766446431354</v>
+        <v>43.959531955662413</v>
       </c>
       <c r="P41" s="0">
-        <v>59.918759272660409</v>
+        <v>64.777571457735448</v>
       </c>
       <c r="Q41" s="0">
-        <v>21.035766353192841</v>
+        <v>15.103410376999443</v>
       </c>
     </row>
     <row r="42">
@@ -2311,7 +2321,7 @@
         <v>4</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="D42" s="0">
         <v>8</v>
@@ -2320,40 +2330,40 @@
         <v>4</v>
       </c>
       <c r="F42" s="0">
-        <v>33.25</v>
+        <v>22.75</v>
       </c>
       <c r="G42" s="0">
-        <v>5.1051444641655346</v>
+        <v>3.6827299656640586</v>
       </c>
       <c r="H42" s="0">
-        <v>7.5</v>
+        <v>8.75</v>
       </c>
       <c r="I42" s="0">
-        <v>2.5331140255951108</v>
+        <v>2.6887109674836132</v>
       </c>
       <c r="J42" s="0">
-        <v>25.75</v>
+        <v>15.25</v>
       </c>
       <c r="K42" s="0">
-        <v>3.6371921404658658</v>
+        <v>2.2126530078919591</v>
       </c>
       <c r="L42" s="0">
-        <v>24.25</v>
+        <v>47</v>
       </c>
       <c r="M42" s="0">
-        <v>4.7147817199385456</v>
+        <v>12.935738607954837</v>
       </c>
       <c r="N42" s="0">
-        <v>142.98126893939397</v>
+        <v>157.92080176767675</v>
       </c>
       <c r="O42" s="0">
-        <v>36.959966323550475</v>
+        <v>83.227737171056702</v>
       </c>
       <c r="P42" s="0">
-        <v>75.952174842019758</v>
+        <v>50.256551304898892</v>
       </c>
       <c r="Q42" s="0">
-        <v>10.026028158088602</v>
+        <v>7.7511695070748141</v>
       </c>
     </row>
     <row r="43">
@@ -2364,7 +2374,7 @@
         <v>4</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="D43" s="0">
         <v>9</v>
@@ -2373,40 +2383,40 @@
         <v>4</v>
       </c>
       <c r="F43" s="0">
-        <v>17.25</v>
+        <v>29.5</v>
       </c>
       <c r="G43" s="0">
-        <v>4.732423621500228</v>
+        <v>4.1733280085163047</v>
       </c>
       <c r="H43" s="0">
-        <v>9.25</v>
+        <v>5.75</v>
       </c>
       <c r="I43" s="0">
-        <v>6.9686799323831767</v>
+        <v>1.4930394055974097</v>
       </c>
       <c r="J43" s="0">
-        <v>14.25</v>
+        <v>19.75</v>
       </c>
       <c r="K43" s="0">
-        <v>4.4040700872412701</v>
+        <v>2.2867371223353739</v>
       </c>
       <c r="L43" s="0">
-        <v>31</v>
+        <v>50.75</v>
       </c>
       <c r="M43" s="0">
-        <v>18.605554726120548</v>
+        <v>16.131620088096131</v>
       </c>
       <c r="N43" s="0">
-        <v>306.30527777777775</v>
+        <v>65.46980357142867</v>
       </c>
       <c r="O43" s="0">
-        <v>144.64282161794904</v>
+        <v>42.191087062516566</v>
       </c>
       <c r="P43" s="0">
-        <v>42.255216679264713</v>
+        <v>64.147899335807864</v>
       </c>
       <c r="Q43" s="0">
-        <v>13.15467278835462</v>
+        <v>5.9704849097917378</v>
       </c>
     </row>
     <row r="44">
@@ -2417,7 +2427,7 @@
         <v>4</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="D44" s="0">
         <v>10</v>
@@ -2426,40 +2436,40 @@
         <v>4</v>
       </c>
       <c r="F44" s="0">
-        <v>16.25</v>
+        <v>26.25</v>
       </c>
       <c r="G44" s="0">
-        <v>5.5733742024019888</v>
+        <v>6.3688696014284982</v>
       </c>
       <c r="H44" s="0">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I44" s="0">
-        <v>0.57735026918962573</v>
+        <v>1.2909944487358056</v>
       </c>
       <c r="J44" s="0">
-        <v>11.25</v>
+        <v>19.5</v>
       </c>
       <c r="K44" s="0">
-        <v>3.7052890125692848</v>
+        <v>4.4253060157839181</v>
       </c>
       <c r="L44" s="0">
-        <v>19</v>
+        <v>52.25</v>
       </c>
       <c r="M44" s="0">
-        <v>3.7638632635454048</v>
+        <v>7.3979163733220625</v>
       </c>
       <c r="N44" s="0">
-        <v>180.63086507936512</v>
+        <v>76.725373376623381</v>
       </c>
       <c r="O44" s="0">
-        <v>56.827780897825768</v>
+        <v>69.106430857045268</v>
       </c>
       <c r="P44" s="0">
-        <v>33.331271553867516</v>
+        <v>63.31241883365562</v>
       </c>
       <c r="Q44" s="0">
-        <v>10.908418051016014</v>
+        <v>13.870452293565409</v>
       </c>
     </row>
     <row r="45">
@@ -2470,7 +2480,7 @@
         <v>4</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="D45" s="0">
         <v>11</v>
@@ -2479,40 +2489,1088 @@
         <v>4</v>
       </c>
       <c r="F45" s="0">
+        <v>25.75</v>
+      </c>
+      <c r="G45" s="0">
+        <v>3.966001344763598</v>
+      </c>
+      <c r="H45" s="0">
+        <v>4.5</v>
+      </c>
+      <c r="I45" s="0">
+        <v>1.9364916731037085</v>
+      </c>
+      <c r="J45" s="0">
         <v>20.25</v>
       </c>
-      <c r="G45" s="0">
+      <c r="K45" s="0">
+        <v>2.0155644370746373</v>
+      </c>
+      <c r="L45" s="0">
+        <v>48.25</v>
+      </c>
+      <c r="M45" s="0">
+        <v>11.360567767501763</v>
+      </c>
+      <c r="N45" s="0">
+        <v>51.138666666666744</v>
+      </c>
+      <c r="O45" s="0">
+        <v>40.114655891304643</v>
+      </c>
+      <c r="P45" s="0">
+        <v>64.238335695371177</v>
+      </c>
+      <c r="Q45" s="0">
+        <v>4.4645526493660395</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D46" s="0">
+        <v>12</v>
+      </c>
+      <c r="E46" s="0">
+        <v>4</v>
+      </c>
+      <c r="F46" s="0">
+        <v>42.75</v>
+      </c>
+      <c r="G46" s="0">
+        <v>10.019772119830536</v>
+      </c>
+      <c r="H46" s="0">
+        <v>5</v>
+      </c>
+      <c r="I46" s="0">
+        <v>1.6329931618554521</v>
+      </c>
+      <c r="J46" s="0">
+        <v>28.75</v>
+      </c>
+      <c r="K46" s="0">
+        <v>5.7789128158619363</v>
+      </c>
+      <c r="L46" s="0">
+        <v>44.75</v>
+      </c>
+      <c r="M46" s="0">
+        <v>5.7644745351737541</v>
+      </c>
+      <c r="N46" s="0">
+        <v>25.704719336219309</v>
+      </c>
+      <c r="O46" s="0">
+        <v>15.641396975578967</v>
+      </c>
+      <c r="P46" s="0">
+        <v>94.175646488409257</v>
+      </c>
+      <c r="Q46" s="0">
+        <v>23.051089999527441</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D47" s="0">
+        <v>13</v>
+      </c>
+      <c r="E47" s="0">
+        <v>4</v>
+      </c>
+      <c r="F47" s="0">
+        <v>32.75</v>
+      </c>
+      <c r="G47" s="0">
+        <v>3.0652623596249202</v>
+      </c>
+      <c r="H47" s="0">
+        <v>10.75</v>
+      </c>
+      <c r="I47" s="0">
+        <v>3.727711541057507</v>
+      </c>
+      <c r="J47" s="0">
+        <v>24.75</v>
+      </c>
+      <c r="K47" s="0">
+        <v>1.796988221070652</v>
+      </c>
+      <c r="L47" s="0">
+        <v>56.25</v>
+      </c>
+      <c r="M47" s="0">
+        <v>15.195256935416833</v>
+      </c>
+      <c r="N47" s="0">
+        <v>28.258526785714359</v>
+      </c>
+      <c r="O47" s="0">
+        <v>9.0461220240131937</v>
+      </c>
+      <c r="P47" s="0">
+        <v>79.812837679384813</v>
+      </c>
+      <c r="Q47" s="0">
+        <v>8.992374134090074</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D48" s="0">
+        <v>14</v>
+      </c>
+      <c r="E48" s="0">
+        <v>4</v>
+      </c>
+      <c r="F48" s="0">
+        <v>37</v>
+      </c>
+      <c r="G48" s="0">
+        <v>1.9578900207451218</v>
+      </c>
+      <c r="H48" s="0">
+        <v>6.5</v>
+      </c>
+      <c r="I48" s="0">
+        <v>1.2583057392117916</v>
+      </c>
+      <c r="J48" s="0">
+        <v>23.25</v>
+      </c>
+      <c r="K48" s="0">
+        <v>2.3228933107943921</v>
+      </c>
+      <c r="L48" s="0">
+        <v>40.25</v>
+      </c>
+      <c r="M48" s="0">
+        <v>11.145813862911343</v>
+      </c>
+      <c r="N48" s="0">
+        <v>47.795265700483078</v>
+      </c>
+      <c r="O48" s="0">
+        <v>27.238849941220227</v>
+      </c>
+      <c r="P48" s="0">
+        <v>73.660580051462745</v>
+      </c>
+      <c r="Q48" s="0">
+        <v>5.450846864686576</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C49" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D49" s="0">
+        <v>15</v>
+      </c>
+      <c r="E49" s="0">
+        <v>4</v>
+      </c>
+      <c r="F49" s="0">
+        <v>27.5</v>
+      </c>
+      <c r="G49" s="0">
+        <v>3.7969285832981723</v>
+      </c>
+      <c r="H49" s="0">
+        <v>4.75</v>
+      </c>
+      <c r="I49" s="0">
+        <v>1.25</v>
+      </c>
+      <c r="J49" s="0">
+        <v>18.75</v>
+      </c>
+      <c r="K49" s="0">
+        <v>3.6371921404658658</v>
+      </c>
+      <c r="L49" s="0">
+        <v>44.25</v>
+      </c>
+      <c r="M49" s="0">
+        <v>11.778334630441888</v>
+      </c>
+      <c r="N49" s="0">
+        <v>88.2486706349207</v>
+      </c>
+      <c r="O49" s="0">
+        <v>51.947599644891973</v>
+      </c>
+      <c r="P49" s="0">
+        <v>58.745823293261395</v>
+      </c>
+      <c r="Q49" s="0">
+        <v>9.2946014595546824</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B50" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C50" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D50" s="0">
+        <v>0</v>
+      </c>
+      <c r="E50" s="0">
+        <v>4</v>
+      </c>
+      <c r="F50" s="0">
+        <v>11.5</v>
+      </c>
+      <c r="G50" s="0">
+        <v>3.378855822118882</v>
+      </c>
+      <c r="H50" s="0">
+        <v>5.75</v>
+      </c>
+      <c r="I50" s="0">
+        <v>1.1086778913041726</v>
+      </c>
+      <c r="J50" s="0">
+        <v>6.75</v>
+      </c>
+      <c r="K50" s="0">
+        <v>1.973786547054502</v>
+      </c>
+      <c r="L50" s="0">
+        <v>26.75</v>
+      </c>
+      <c r="M50" s="0">
+        <v>2.5289984842489197</v>
+      </c>
+      <c r="N50" s="0"/>
+      <c r="O50" s="0"/>
+      <c r="P50" s="0">
+        <v>0</v>
+      </c>
+      <c r="Q50" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C51" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D51" s="0">
+        <v>1</v>
+      </c>
+      <c r="E51" s="0">
+        <v>4</v>
+      </c>
+      <c r="F51" s="0">
+        <v>29.75</v>
+      </c>
+      <c r="G51" s="0">
+        <v>12.51915199471061</v>
+      </c>
+      <c r="H51" s="0">
+        <v>5.5</v>
+      </c>
+      <c r="I51" s="0">
+        <v>2.5331140255951108</v>
+      </c>
+      <c r="J51" s="0">
+        <v>18</v>
+      </c>
+      <c r="K51" s="0">
+        <v>6.324555320336759</v>
+      </c>
+      <c r="L51" s="0">
+        <v>49.75</v>
+      </c>
+      <c r="M51" s="0">
+        <v>11.678862672937521</v>
+      </c>
+      <c r="N51" s="0">
+        <v>199.02467307692302</v>
+      </c>
+      <c r="O51" s="0">
+        <v>83.158139318497049</v>
+      </c>
+      <c r="P51" s="0">
+        <v>65535</v>
+      </c>
+      <c r="Q51" s="0"/>
+    </row>
+    <row r="52">
+      <c r="A52" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B52" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C52" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D52" s="0">
+        <v>2</v>
+      </c>
+      <c r="E52" s="0">
+        <v>4</v>
+      </c>
+      <c r="F52" s="0">
+        <v>28.5</v>
+      </c>
+      <c r="G52" s="0">
+        <v>8.4606934309980364</v>
+      </c>
+      <c r="H52" s="0">
+        <v>4.5</v>
+      </c>
+      <c r="I52" s="0">
+        <v>1.0408329997330663</v>
+      </c>
+      <c r="J52" s="0">
+        <v>18.25</v>
+      </c>
+      <c r="K52" s="0">
+        <v>5.5283360968739954</v>
+      </c>
+      <c r="L52" s="0">
+        <v>16.5</v>
+      </c>
+      <c r="M52" s="0">
+        <v>4.0926763859362252</v>
+      </c>
+      <c r="N52" s="0">
+        <v>123.76519444444445</v>
+      </c>
+      <c r="O52" s="0">
+        <v>96.563654110602727</v>
+      </c>
+      <c r="P52" s="0">
+        <v>57.096024507691922</v>
+      </c>
+      <c r="Q52" s="0">
+        <v>17.581199231611976</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B53" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C53" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D53" s="0">
+        <v>3</v>
+      </c>
+      <c r="E53" s="0">
+        <v>4</v>
+      </c>
+      <c r="F53" s="0">
+        <v>54.25</v>
+      </c>
+      <c r="G53" s="0">
+        <v>23.264332499916403</v>
+      </c>
+      <c r="H53" s="0">
+        <v>12</v>
+      </c>
+      <c r="I53" s="0">
+        <v>5.8166427888717163</v>
+      </c>
+      <c r="J53" s="0">
+        <v>37</v>
+      </c>
+      <c r="K53" s="0">
+        <v>16.416455159382004</v>
+      </c>
+      <c r="L53" s="0">
+        <v>29.25</v>
+      </c>
+      <c r="M53" s="0">
+        <v>7.1922991224410753</v>
+      </c>
+      <c r="N53" s="0">
+        <v>396.74887121212117</v>
+      </c>
+      <c r="O53" s="0">
+        <v>320.97552634128039</v>
+      </c>
+      <c r="P53" s="0">
+        <v>65535</v>
+      </c>
+      <c r="Q53" s="0"/>
+    </row>
+    <row r="54">
+      <c r="A54" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B54" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D54" s="0">
+        <v>4</v>
+      </c>
+      <c r="E54" s="0">
+        <v>4</v>
+      </c>
+      <c r="F54" s="0">
+        <v>37.25</v>
+      </c>
+      <c r="G54" s="0">
+        <v>15.939338129295081</v>
+      </c>
+      <c r="H54" s="0">
+        <v>5.75</v>
+      </c>
+      <c r="I54" s="0">
+        <v>2.462214450449026</v>
+      </c>
+      <c r="J54" s="0">
+        <v>30.5</v>
+      </c>
+      <c r="K54" s="0">
+        <v>12.038133853162901</v>
+      </c>
+      <c r="L54" s="0">
+        <v>24.25</v>
+      </c>
+      <c r="M54" s="0">
+        <v>8.3404136588061384</v>
+      </c>
+      <c r="N54" s="0">
+        <v>134.40125000000003</v>
+      </c>
+      <c r="O54" s="0">
+        <v>67.057948079527264</v>
+      </c>
+      <c r="P54" s="0">
+        <v>95.023410332767327</v>
+      </c>
+      <c r="Q54" s="0">
+        <v>36.817250218707393</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B55" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C55" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D55" s="0">
+        <v>5</v>
+      </c>
+      <c r="E55" s="0">
+        <v>2</v>
+      </c>
+      <c r="F55" s="0">
+        <v>50.5</v>
+      </c>
+      <c r="G55" s="0">
+        <v>45.499999999999993</v>
+      </c>
+      <c r="H55" s="0">
+        <v>4</v>
+      </c>
+      <c r="I55" s="0">
+        <v>2.9999999999999996</v>
+      </c>
+      <c r="J55" s="0">
+        <v>39</v>
+      </c>
+      <c r="K55" s="0">
+        <v>33.999999999999993</v>
+      </c>
+      <c r="L55" s="0">
+        <v>15.5</v>
+      </c>
+      <c r="M55" s="0">
+        <v>7.5</v>
+      </c>
+      <c r="N55" s="0">
+        <v>587.1704545454545</v>
+      </c>
+      <c r="O55" s="0">
+        <v>570.04954545454541</v>
+      </c>
+      <c r="P55" s="0">
+        <v>120.13736051271005</v>
+      </c>
+      <c r="Q55" s="0">
+        <v>104.12195766910814</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B56" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C56" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D56" s="0">
+        <v>6</v>
+      </c>
+      <c r="E56" s="0">
+        <v>4</v>
+      </c>
+      <c r="F56" s="0">
+        <v>26</v>
+      </c>
+      <c r="G56" s="0">
+        <v>9.9582461641931044</v>
+      </c>
+      <c r="H56" s="0">
+        <v>6.75</v>
+      </c>
+      <c r="I56" s="0">
+        <v>2.6575364531836625</v>
+      </c>
+      <c r="J56" s="0">
+        <v>20.75</v>
+      </c>
+      <c r="K56" s="0">
+        <v>8.1687922403906601</v>
+      </c>
+      <c r="L56" s="0">
+        <v>22.5</v>
+      </c>
+      <c r="M56" s="0">
+        <v>4.1932485418030412</v>
+      </c>
+      <c r="N56" s="0">
+        <v>347.29934920634918</v>
+      </c>
+      <c r="O56" s="0">
+        <v>158.54349546179873</v>
+      </c>
+      <c r="P56" s="0">
+        <v>65535</v>
+      </c>
+      <c r="Q56" s="0"/>
+    </row>
+    <row r="57">
+      <c r="A57" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B57" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C57" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D57" s="0">
+        <v>7</v>
+      </c>
+      <c r="E57" s="0">
+        <v>4</v>
+      </c>
+      <c r="F57" s="0">
+        <v>22.75</v>
+      </c>
+      <c r="G57" s="0">
+        <v>7.9621500446382782</v>
+      </c>
+      <c r="H57" s="0">
+        <v>3.75</v>
+      </c>
+      <c r="I57" s="0">
+        <v>1.6520189667999174</v>
+      </c>
+      <c r="J57" s="0">
+        <v>20.25</v>
+      </c>
+      <c r="K57" s="0">
+        <v>7.2154348448309058</v>
+      </c>
+      <c r="L57" s="0">
+        <v>22.75</v>
+      </c>
+      <c r="M57" s="0">
+        <v>7.9201746613737418</v>
+      </c>
+      <c r="N57" s="0">
+        <v>708.12724358974367</v>
+      </c>
+      <c r="O57" s="0">
+        <v>561.21766446431354</v>
+      </c>
+      <c r="P57" s="0">
+        <v>59.918759272660409</v>
+      </c>
+      <c r="Q57" s="0">
+        <v>21.035766353192841</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B58" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C58" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D58" s="0">
+        <v>8</v>
+      </c>
+      <c r="E58" s="0">
+        <v>4</v>
+      </c>
+      <c r="F58" s="0">
+        <v>33.25</v>
+      </c>
+      <c r="G58" s="0">
+        <v>5.1051444641655346</v>
+      </c>
+      <c r="H58" s="0">
+        <v>7.5</v>
+      </c>
+      <c r="I58" s="0">
+        <v>2.5331140255951108</v>
+      </c>
+      <c r="J58" s="0">
+        <v>25.75</v>
+      </c>
+      <c r="K58" s="0">
+        <v>3.6371921404658658</v>
+      </c>
+      <c r="L58" s="0">
+        <v>24.25</v>
+      </c>
+      <c r="M58" s="0">
+        <v>4.7147817199385456</v>
+      </c>
+      <c r="N58" s="0">
+        <v>142.98126893939397</v>
+      </c>
+      <c r="O58" s="0">
+        <v>36.959966323550475</v>
+      </c>
+      <c r="P58" s="0">
+        <v>75.952174842019758</v>
+      </c>
+      <c r="Q58" s="0">
+        <v>10.026028158088602</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B59" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C59" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D59" s="0">
+        <v>9</v>
+      </c>
+      <c r="E59" s="0">
+        <v>4</v>
+      </c>
+      <c r="F59" s="0">
+        <v>17.25</v>
+      </c>
+      <c r="G59" s="0">
+        <v>4.732423621500228</v>
+      </c>
+      <c r="H59" s="0">
+        <v>9.25</v>
+      </c>
+      <c r="I59" s="0">
+        <v>6.9686799323831767</v>
+      </c>
+      <c r="J59" s="0">
+        <v>14.25</v>
+      </c>
+      <c r="K59" s="0">
+        <v>4.4040700872412701</v>
+      </c>
+      <c r="L59" s="0">
+        <v>31</v>
+      </c>
+      <c r="M59" s="0">
+        <v>18.605554726120548</v>
+      </c>
+      <c r="N59" s="0">
+        <v>306.30527777777775</v>
+      </c>
+      <c r="O59" s="0">
+        <v>144.64282161794904</v>
+      </c>
+      <c r="P59" s="0">
+        <v>42.255216679264713</v>
+      </c>
+      <c r="Q59" s="0">
+        <v>13.15467278835462</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B60" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C60" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D60" s="0">
+        <v>10</v>
+      </c>
+      <c r="E60" s="0">
+        <v>4</v>
+      </c>
+      <c r="F60" s="0">
+        <v>16.25</v>
+      </c>
+      <c r="G60" s="0">
+        <v>5.5733742024019888</v>
+      </c>
+      <c r="H60" s="0">
+        <v>1</v>
+      </c>
+      <c r="I60" s="0">
+        <v>0.57735026918962573</v>
+      </c>
+      <c r="J60" s="0">
+        <v>11.25</v>
+      </c>
+      <c r="K60" s="0">
+        <v>3.7052890125692848</v>
+      </c>
+      <c r="L60" s="0">
+        <v>19</v>
+      </c>
+      <c r="M60" s="0">
+        <v>3.7638632635454048</v>
+      </c>
+      <c r="N60" s="0">
+        <v>180.63086507936512</v>
+      </c>
+      <c r="O60" s="0">
+        <v>56.827780897825768</v>
+      </c>
+      <c r="P60" s="0">
+        <v>33.331271553867516</v>
+      </c>
+      <c r="Q60" s="0">
+        <v>10.908418051016014</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B61" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C61" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D61" s="0">
+        <v>11</v>
+      </c>
+      <c r="E61" s="0">
+        <v>4</v>
+      </c>
+      <c r="F61" s="0">
+        <v>20.25</v>
+      </c>
+      <c r="G61" s="0">
         <v>4.3851073723076235</v>
       </c>
-      <c r="H45" s="0">
+      <c r="H61" s="0">
         <v>6.25</v>
       </c>
-      <c r="I45" s="0">
+      <c r="I61" s="0">
         <v>0.8539125638299665</v>
       </c>
-      <c r="J45" s="0">
+      <c r="J61" s="0">
         <v>14.75</v>
       </c>
-      <c r="K45" s="0">
+      <c r="K61" s="0">
         <v>3.4247870980057527</v>
       </c>
-      <c r="L45" s="0">
+      <c r="L61" s="0">
         <v>28.25</v>
       </c>
-      <c r="M45" s="0">
+      <c r="M61" s="0">
         <v>3.2755406678389241</v>
       </c>
-      <c r="N45" s="0">
+      <c r="N61" s="0">
         <v>37.815684210526243</v>
       </c>
-      <c r="O45" s="0">
+      <c r="O61" s="0">
         <v>1.8994763552843577</v>
       </c>
-      <c r="P45" s="0">
+      <c r="P61" s="0">
         <v>42.611982644485956</v>
       </c>
-      <c r="Q45" s="0">
+      <c r="Q61" s="0">
         <v>9.8438187406455917</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B62" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C62" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D62" s="0">
+        <v>12</v>
+      </c>
+      <c r="E62" s="0">
+        <v>4</v>
+      </c>
+      <c r="F62" s="0">
+        <v>16.25</v>
+      </c>
+      <c r="G62" s="0">
+        <v>6.472699076377129</v>
+      </c>
+      <c r="H62" s="0">
+        <v>2.25</v>
+      </c>
+      <c r="I62" s="0">
+        <v>0.75</v>
+      </c>
+      <c r="J62" s="0">
+        <v>13.25</v>
+      </c>
+      <c r="K62" s="0">
+        <v>6.0190669265814503</v>
+      </c>
+      <c r="L62" s="0">
+        <v>38</v>
+      </c>
+      <c r="M62" s="0">
+        <v>10.230672835481871</v>
+      </c>
+      <c r="N62" s="0">
+        <v>192.07601190476191</v>
+      </c>
+      <c r="O62" s="0">
+        <v>142.6828567917467</v>
+      </c>
+      <c r="P62" s="0">
+        <v>65535</v>
+      </c>
+      <c r="Q62" s="0"/>
+    </row>
+    <row r="63">
+      <c r="A63" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B63" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C63" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D63" s="0">
+        <v>13</v>
+      </c>
+      <c r="E63" s="0">
+        <v>4</v>
+      </c>
+      <c r="F63" s="0">
+        <v>22.25</v>
+      </c>
+      <c r="G63" s="0">
+        <v>7.6634957210575037</v>
+      </c>
+      <c r="H63" s="0">
+        <v>3</v>
+      </c>
+      <c r="I63" s="0">
+        <v>0.40824829046386302</v>
+      </c>
+      <c r="J63" s="0">
+        <v>19</v>
+      </c>
+      <c r="K63" s="0">
+        <v>6.8920243760451108</v>
+      </c>
+      <c r="L63" s="0">
+        <v>55</v>
+      </c>
+      <c r="M63" s="0">
+        <v>21.459263733874934</v>
+      </c>
+      <c r="N63" s="0">
+        <v>615.06807878151267</v>
+      </c>
+      <c r="O63" s="0">
+        <v>460.5257697598081</v>
+      </c>
+      <c r="P63" s="0">
+        <v>54.455336742364189</v>
+      </c>
+      <c r="Q63" s="0">
+        <v>19.576332030120021</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B64" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C64" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D64" s="0">
+        <v>14</v>
+      </c>
+      <c r="E64" s="0">
+        <v>4</v>
+      </c>
+      <c r="F64" s="0">
+        <v>21</v>
+      </c>
+      <c r="G64" s="0">
+        <v>8.755950357709132</v>
+      </c>
+      <c r="H64" s="0">
+        <v>2.75</v>
+      </c>
+      <c r="I64" s="0">
+        <v>0.62915286960589578</v>
+      </c>
+      <c r="J64" s="0">
+        <v>17.25</v>
+      </c>
+      <c r="K64" s="0">
+        <v>7.8885465496925775</v>
+      </c>
+      <c r="L64" s="0">
+        <v>53.75</v>
+      </c>
+      <c r="M64" s="0">
+        <v>23.792068005955262</v>
+      </c>
+      <c r="N64" s="0">
+        <v>112.15200541795659</v>
+      </c>
+      <c r="O64" s="0">
+        <v>71.500120010883265</v>
+      </c>
+      <c r="P64" s="0">
+        <v>49.359967524618412</v>
+      </c>
+      <c r="Q64" s="0">
+        <v>22.448608149749454</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B65" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C65" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D65" s="0">
+        <v>15</v>
+      </c>
+      <c r="E65" s="0">
+        <v>4</v>
+      </c>
+      <c r="F65" s="0">
+        <v>26</v>
+      </c>
+      <c r="G65" s="0">
+        <v>13.310396938734272</v>
+      </c>
+      <c r="H65" s="0">
+        <v>3.75</v>
+      </c>
+      <c r="I65" s="0">
+        <v>1.4930394055974097</v>
+      </c>
+      <c r="J65" s="0">
+        <v>18.5</v>
+      </c>
+      <c r="K65" s="0">
+        <v>8.9116029235298999</v>
+      </c>
+      <c r="L65" s="0">
+        <v>43.25</v>
+      </c>
+      <c r="M65" s="0">
+        <v>16.064323826417343</v>
+      </c>
+      <c r="N65" s="0">
+        <v>28.478772522522533</v>
+      </c>
+      <c r="O65" s="0">
+        <v>12.265467204347953</v>
+      </c>
+      <c r="P65" s="0">
+        <v>52.883651201847584</v>
+      </c>
+      <c r="Q65" s="0">
+        <v>25.424951259661405</v>
       </c>
     </row>
   </sheetData>

</xml_diff>